<commit_message>
REF: fill order and addresses
</commit_message>
<xml_diff>
--- a/build-PSS_HomeWork4-Desktop_Qt_5_12_5_MinGW_64_bit-Release/release/DataBase/Accounts.xlsx
+++ b/build-PSS_HomeWork4-Desktop_Qt_5_12_5_MinGW_64_bit-Release/release/DataBase/Accounts.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="15444" yWindow="-12" windowWidth="15312" windowHeight="13980" activeTab="2"/>
+    <workbookView xWindow="15444" yWindow="-12" windowWidth="15312" windowHeight="13980" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Passenger" sheetId="1" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="272">
   <si>
     <t>James</t>
   </si>
@@ -883,6 +883,19 @@
   </si>
   <si>
     <t>608 Ondricka Crossing Skilesbury, MA 45237</t>
+  </si>
+  <si>
+    <t>Home</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+3716 Donnelly Common Rathton, ME 32302</t>
+  </si>
+  <si>
+    <t>1655 Garry Cape Ednamouth, VT 32471</t>
+  </si>
+  <si>
+    <t>Work</t>
   </si>
 </sst>
 </file>
@@ -1043,7 +1056,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1064,6 +1077,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -2552,9 +2566,11 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
@@ -2567,6 +2583,21 @@
       </c>
       <c r="C1" s="4" t="s">
         <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -2576,9 +2607,11 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
@@ -2591,6 +2624,21 @@
       </c>
       <c r="C1" s="4" t="s">
         <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -2600,9 +2648,11 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
@@ -2615,6 +2665,21 @@
       </c>
       <c r="C1" s="4" t="s">
         <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -2624,9 +2689,11 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
@@ -2639,6 +2706,21 @@
       </c>
       <c r="C1" s="4" t="s">
         <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -2648,9 +2730,11 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
@@ -2663,6 +2747,21 @@
       </c>
       <c r="C1" s="4" t="s">
         <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -2672,9 +2771,11 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
@@ -2687,6 +2788,21 @@
       </c>
       <c r="C1" s="4" t="s">
         <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -2696,9 +2812,11 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
@@ -2711,6 +2829,21 @@
       </c>
       <c r="C1" s="4" t="s">
         <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -2720,9 +2853,11 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
@@ -2735,6 +2870,21 @@
       </c>
       <c r="C1" s="4" t="s">
         <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -2744,9 +2894,11 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
@@ -2759,6 +2911,21 @@
       </c>
       <c r="C1" s="4" t="s">
         <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -2768,9 +2935,11 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
@@ -2783,6 +2952,21 @@
       </c>
       <c r="C1" s="4" t="s">
         <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -2991,9 +3175,11 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
@@ -3006,6 +3192,21 @@
       </c>
       <c r="C1" s="4" t="s">
         <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -3015,9 +3216,11 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
@@ -3030,6 +3233,21 @@
       </c>
       <c r="C1" s="4" t="s">
         <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -3039,9 +3257,11 @@
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
@@ -3054,6 +3274,26 @@
       </c>
       <c r="C1" s="4" t="s">
         <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -3063,9 +3303,11 @@
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
@@ -3078,6 +3320,26 @@
       </c>
       <c r="C1" s="4" t="s">
         <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -3087,9 +3349,11 @@
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
@@ -3102,6 +3366,21 @@
       </c>
       <c r="C1" s="4" t="s">
         <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -3111,9 +3390,11 @@
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
@@ -3126,6 +3407,16 @@
       </c>
       <c r="C1" s="4" t="s">
         <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -3135,9 +3426,11 @@
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="E47" sqref="E47"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
@@ -3150,6 +3443,21 @@
       </c>
       <c r="C1" s="4" t="s">
         <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -3159,9 +3467,11 @@
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
@@ -3174,6 +3484,16 @@
       </c>
       <c r="C1" s="4" t="s">
         <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -3183,9 +3503,11 @@
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
@@ -3198,6 +3520,16 @@
       </c>
       <c r="C1" s="4" t="s">
         <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -3207,9 +3539,11 @@
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="J47" sqref="J47"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
@@ -3222,6 +3556,11 @@
       </c>
       <c r="C1" s="4" t="s">
         <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -3233,8 +3572,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L39" sqref="L39"/>
+    <sheetView topLeftCell="A46" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3462,7 +3801,7 @@
       <c r="G8" s="2">
         <v>44169</v>
       </c>
-      <c r="I8" s="13" t="s">
+      <c r="H8" s="13" t="s">
         <v>143</v>
       </c>
     </row>
@@ -5084,9 +5423,11 @@
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
@@ -5099,6 +5440,11 @@
       </c>
       <c r="C1" s="4" t="s">
         <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -5108,9 +5454,11 @@
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
@@ -5123,6 +5471,11 @@
       </c>
       <c r="C1" s="4" t="s">
         <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -5132,9 +5485,11 @@
 
 <file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
@@ -5147,6 +5502,11 @@
       </c>
       <c r="C1" s="4" t="s">
         <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -5156,9 +5516,11 @@
 
 <file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
@@ -5171,6 +5533,11 @@
       </c>
       <c r="C1" s="4" t="s">
         <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -5180,9 +5547,11 @@
 
 <file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
@@ -5195,6 +5564,11 @@
       </c>
       <c r="C1" s="4" t="s">
         <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -5204,9 +5578,11 @@
 
 <file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
@@ -5219,6 +5595,11 @@
       </c>
       <c r="C1" s="4" t="s">
         <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -5228,9 +5609,11 @@
 
 <file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
@@ -5243,6 +5626,11 @@
       </c>
       <c r="C1" s="4" t="s">
         <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -5252,9 +5640,11 @@
 
 <file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
@@ -5267,6 +5657,16 @@
       </c>
       <c r="C1" s="4" t="s">
         <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -5327,7 +5727,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -5346,6 +5746,12 @@
     <row r="2" spans="1:3">
       <c r="A2">
         <v>1</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>269</v>
+      </c>
+      <c r="C2" t="s">
+        <v>268</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -5362,7 +5768,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="F47" sqref="F47"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
@@ -5552,9 +5960,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
@@ -5567,6 +5977,22 @@
       </c>
       <c r="C1" s="4" t="s">
         <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>270</v>
+      </c>
+      <c r="C2" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -5576,9 +6002,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
@@ -5591,6 +6019,26 @@
       </c>
       <c r="C1" s="4" t="s">
         <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -5600,9 +6048,11 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
@@ -5615,6 +6065,11 @@
       </c>
       <c r="C1" s="4" t="s">
         <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -5624,9 +6079,11 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
@@ -5639,6 +6096,11 @@
       </c>
       <c r="C1" s="4" t="s">
         <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -5648,9 +6110,11 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
@@ -5665,6 +6129,11 @@
         <v>101</v>
       </c>
     </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
ADD: class user as a layer ADD: taking data about passenger from database ADD: implementation of Address and Order
REF(interface): PrintInfo -> menu

DEL: peoplegenerator -> database
</commit_message>
<xml_diff>
--- a/build-PSS_HomeWork4-Desktop_Qt_5_12_5_MinGW_64_bit-Release/release/DataBase/Accounts.xlsx
+++ b/build-PSS_HomeWork4-Desktop_Qt_5_12_5_MinGW_64_bit-Release/release/DataBase/Accounts.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="15444" yWindow="-12" windowWidth="15312" windowHeight="13980" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Passenger" sheetId="1" r:id="rId1"/>
@@ -422,7 +422,6 @@
         <color rgb="FF800080"/>
         <rFont val="Arial Unicode MS"/>
         <family val="2"/>
-        <charset val="204"/>
       </rPr>
       <t>Economy</t>
     </r>
@@ -432,7 +431,6 @@
         <color rgb="FFC0C0C0"/>
         <rFont val="Arial Unicode MS"/>
         <family val="2"/>
-        <charset val="204"/>
       </rPr>
       <t/>
     </r>
@@ -888,21 +886,20 @@
     <t>Home</t>
   </si>
   <si>
-    <t xml:space="preserve">
-3716 Donnelly Common Rathton, ME 32302</t>
-  </si>
-  <si>
     <t>1655 Garry Cape Ednamouth, VT 32471</t>
   </si>
   <si>
     <t>Work</t>
+  </si>
+  <si>
+    <t>3716 Donnelly Common Rathton, ME 32302</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -933,6 +930,18 @@
       <family val="2"/>
       <charset val="204"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF800080"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFC0C0C0"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1056,7 +1065,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1077,6 +1086,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -1374,9 +1384,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19:D25"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
@@ -2568,9 +2576,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
+    <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
@@ -2609,9 +2615,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
-    </sheetView>
+    <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
@@ -2650,9 +2654,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
+    <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
@@ -2691,9 +2693,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
+    <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
@@ -2732,9 +2732,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
+    <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
@@ -2773,9 +2771,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
+    <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
@@ -2814,9 +2810,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
+    <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
@@ -2855,9 +2849,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
+    <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
@@ -2896,9 +2888,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
+    <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
@@ -2937,9 +2927,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
+    <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
@@ -3177,9 +3165,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
+    <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
@@ -3218,9 +3204,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
+    <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
@@ -3259,9 +3243,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
-    </sheetView>
+    <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
@@ -3305,9 +3287,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
-    </sheetView>
+    <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
@@ -3351,9 +3331,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
+    <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
@@ -3392,9 +3370,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
+    <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
@@ -3428,9 +3404,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="E47" sqref="E47"/>
-    </sheetView>
+    <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
@@ -3469,9 +3443,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
+    <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
@@ -3505,9 +3477,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
+    <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
@@ -3541,9 +3511,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="J47" sqref="J47"/>
-    </sheetView>
+    <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
@@ -3572,23 +3540,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N78"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.33203125" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" customWidth="1"/>
+    <col min="3" max="3" width="9.5546875" customWidth="1"/>
+    <col min="4" max="4" width="7.77734375" customWidth="1"/>
+    <col min="5" max="5" width="7" customWidth="1"/>
+    <col min="6" max="6" width="8.109375" customWidth="1"/>
+    <col min="7" max="7" width="10.109375" customWidth="1"/>
+    <col min="10" max="10" width="14.33203125" customWidth="1"/>
+    <col min="11" max="11" width="8.77734375" customWidth="1"/>
+    <col min="12" max="12" width="7.6640625" customWidth="1"/>
+    <col min="13" max="13" width="11.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15">
@@ -3629,7 +3595,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="15" thickBot="1">
+    <row r="2" spans="1:14">
       <c r="A2" s="12">
         <v>1</v>
       </c>
@@ -5417,7 +5383,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
 </file>
 
@@ -5425,9 +5391,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
@@ -5456,9 +5420,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
@@ -5487,9 +5449,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
@@ -5518,9 +5478,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
@@ -5549,9 +5507,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
@@ -5580,9 +5536,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
@@ -5611,9 +5565,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
@@ -5642,9 +5594,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
+    <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
@@ -5726,7 +5676,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -5747,8 +5697,8 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="14" t="s">
-        <v>269</v>
+      <c r="B2" s="15" t="s">
+        <v>271</v>
       </c>
       <c r="C2" t="s">
         <v>268</v>
@@ -5768,9 +5718,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="F47" sqref="F47"/>
-    </sheetView>
+    <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
@@ -5962,8 +5910,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -5983,11 +5931,11 @@
       <c r="A2">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="14" t="s">
+        <v>269</v>
+      </c>
+      <c r="C2" t="s">
         <v>270</v>
-      </c>
-      <c r="C2" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -6004,9 +5952,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
-    </sheetView>
+    <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
@@ -6050,9 +5996,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
@@ -6081,9 +6025,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
@@ -6112,9 +6054,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>

</xml_diff>

<commit_message>
MOVE Car class ADD: Driver database ADD: Driver implementation
</commit_message>
<xml_diff>
--- a/build-PSS_HomeWork4-Desktop_Qt_5_12_5_MinGW_64_bit-Release/release/DataBase/Accounts.xlsx
+++ b/build-PSS_HomeWork4-Desktop_Qt_5_12_5_MinGW_64_bit-Release/release/DataBase/Accounts.xlsx
@@ -10,57 +10,64 @@
     <sheet name="Passenger" sheetId="1" r:id="rId1"/>
     <sheet name="Driver" sheetId="2" r:id="rId2"/>
     <sheet name="Orders" sheetId="47" r:id="rId3"/>
-    <sheet name="89959280771" sheetId="3" r:id="rId4"/>
-    <sheet name="89180884879" sheetId="4" r:id="rId5"/>
-    <sheet name="89962840843" sheetId="5" r:id="rId6"/>
-    <sheet name="89313306966" sheetId="6" r:id="rId7"/>
-    <sheet name="89306140496" sheetId="7" r:id="rId8"/>
-    <sheet name="89394702333" sheetId="8" r:id="rId9"/>
-    <sheet name="89833750451" sheetId="9" r:id="rId10"/>
-    <sheet name="89787150096" sheetId="10" r:id="rId11"/>
-    <sheet name="89992098153" sheetId="11" r:id="rId12"/>
-    <sheet name="89268200405" sheetId="12" r:id="rId13"/>
-    <sheet name="89926260702" sheetId="13" r:id="rId14"/>
-    <sheet name="89492911777" sheetId="14" r:id="rId15"/>
-    <sheet name="89330959189" sheetId="15" r:id="rId16"/>
-    <sheet name="89423670770" sheetId="16" r:id="rId17"/>
-    <sheet name="89185241280" sheetId="17" r:id="rId18"/>
-    <sheet name="89990916326" sheetId="18" r:id="rId19"/>
-    <sheet name="89673329996" sheetId="19" r:id="rId20"/>
-    <sheet name="89202864668" sheetId="20" r:id="rId21"/>
-    <sheet name="89601579888" sheetId="21" r:id="rId22"/>
-    <sheet name="89607860943" sheetId="22" r:id="rId23"/>
-    <sheet name="89231886764" sheetId="23" r:id="rId24"/>
-    <sheet name="89539860223" sheetId="24" r:id="rId25"/>
-    <sheet name="89959405648" sheetId="25" r:id="rId26"/>
-    <sheet name="89705356787" sheetId="26" r:id="rId27"/>
-    <sheet name="89832868047" sheetId="27" r:id="rId28"/>
-    <sheet name="89282911827" sheetId="28" r:id="rId29"/>
-    <sheet name="89214352791" sheetId="29" r:id="rId30"/>
-    <sheet name="89133279195" sheetId="30" r:id="rId31"/>
-    <sheet name="89292850692" sheetId="31" r:id="rId32"/>
-    <sheet name="89695933467" sheetId="32" r:id="rId33"/>
-    <sheet name="89278666277" sheetId="33" r:id="rId34"/>
-    <sheet name="89871022956" sheetId="34" r:id="rId35"/>
-    <sheet name="89797832254" sheetId="35" r:id="rId36"/>
-    <sheet name="89281242037" sheetId="36" r:id="rId37"/>
-    <sheet name="89177853860" sheetId="37" r:id="rId38"/>
-    <sheet name="89793704898" sheetId="38" r:id="rId39"/>
-    <sheet name="89624920064" sheetId="39" r:id="rId40"/>
-    <sheet name="89532136828" sheetId="40" r:id="rId41"/>
-    <sheet name="89869988648" sheetId="41" r:id="rId42"/>
-    <sheet name="89767989697" sheetId="42" r:id="rId43"/>
-    <sheet name="89985042567" sheetId="43" r:id="rId44"/>
-    <sheet name="89488486412" sheetId="44" r:id="rId45"/>
-    <sheet name="89297310394" sheetId="45" r:id="rId46"/>
-    <sheet name="89286091054" sheetId="46" r:id="rId47"/>
+    <sheet name="Activ orders" sheetId="54" r:id="rId4"/>
+    <sheet name="89959280771" sheetId="3" r:id="rId5"/>
+    <sheet name="89180884879" sheetId="4" r:id="rId6"/>
+    <sheet name="89962840843" sheetId="5" r:id="rId7"/>
+    <sheet name="89313306966" sheetId="6" r:id="rId8"/>
+    <sheet name="89306140496" sheetId="7" r:id="rId9"/>
+    <sheet name="89394702333" sheetId="8" r:id="rId10"/>
+    <sheet name="89833750451" sheetId="9" r:id="rId11"/>
+    <sheet name="89787150096" sheetId="10" r:id="rId12"/>
+    <sheet name="89992098153" sheetId="11" r:id="rId13"/>
+    <sheet name="89268200405" sheetId="12" r:id="rId14"/>
+    <sheet name="89926260702" sheetId="13" r:id="rId15"/>
+    <sheet name="89492911777" sheetId="14" r:id="rId16"/>
+    <sheet name="89330959189" sheetId="15" r:id="rId17"/>
+    <sheet name="89423670770" sheetId="16" r:id="rId18"/>
+    <sheet name="89185241280" sheetId="17" r:id="rId19"/>
+    <sheet name="89990916326" sheetId="18" r:id="rId20"/>
+    <sheet name="89673329996" sheetId="19" r:id="rId21"/>
+    <sheet name="89202864668" sheetId="20" r:id="rId22"/>
+    <sheet name="89601579888" sheetId="21" r:id="rId23"/>
+    <sheet name="89607860943" sheetId="22" r:id="rId24"/>
+    <sheet name="89231886764" sheetId="23" r:id="rId25"/>
+    <sheet name="89539860223" sheetId="24" r:id="rId26"/>
+    <sheet name="89959405648" sheetId="25" r:id="rId27"/>
+    <sheet name="89705356787" sheetId="26" r:id="rId28"/>
+    <sheet name="89832868047" sheetId="27" r:id="rId29"/>
+    <sheet name="89282911827" sheetId="28" r:id="rId30"/>
+    <sheet name="89214352791" sheetId="29" r:id="rId31"/>
+    <sheet name="89133279195" sheetId="30" r:id="rId32"/>
+    <sheet name="89292850692" sheetId="31" r:id="rId33"/>
+    <sheet name="89695933467" sheetId="32" r:id="rId34"/>
+    <sheet name="89278666277" sheetId="33" r:id="rId35"/>
+    <sheet name="89871022956" sheetId="34" r:id="rId36"/>
+    <sheet name="89797832254" sheetId="35" r:id="rId37"/>
+    <sheet name="89281242037" sheetId="36" r:id="rId38"/>
+    <sheet name="89177853860" sheetId="37" r:id="rId39"/>
+    <sheet name="89793704898" sheetId="38" r:id="rId40"/>
+    <sheet name="89624920064" sheetId="39" r:id="rId41"/>
+    <sheet name="89532136828" sheetId="40" r:id="rId42"/>
+    <sheet name="89869988648" sheetId="41" r:id="rId43"/>
+    <sheet name="89767989697" sheetId="42" r:id="rId44"/>
+    <sheet name="89985042567" sheetId="43" r:id="rId45"/>
+    <sheet name="89488486412" sheetId="44" r:id="rId46"/>
+    <sheet name="89297310394" sheetId="45" r:id="rId47"/>
+    <sheet name="89286091054" sheetId="46" r:id="rId48"/>
+    <sheet name="333223827" sheetId="48" r:id="rId49"/>
+    <sheet name="333223322" sheetId="49" r:id="rId50"/>
+    <sheet name="333225555" sheetId="50" r:id="rId51"/>
+    <sheet name="333221234" sheetId="51" r:id="rId52"/>
+    <sheet name="333227531" sheetId="52" r:id="rId53"/>
+    <sheet name="333220011" sheetId="53" r:id="rId54"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="292">
   <si>
     <t>James</t>
   </si>
@@ -893,6 +900,66 @@
   </si>
   <si>
     <t>3716 Donnelly Common Rathton, ME 32302</t>
+  </si>
+  <si>
+    <t>Car model</t>
+  </si>
+  <si>
+    <t>Car number</t>
+  </si>
+  <si>
+    <t>Lada Granta Sedan</t>
+  </si>
+  <si>
+    <t>H928MK</t>
+  </si>
+  <si>
+    <t>E886CT</t>
+  </si>
+  <si>
+    <t>P427PX</t>
+  </si>
+  <si>
+    <t>X916XA</t>
+  </si>
+  <si>
+    <t>H494ET</t>
+  </si>
+  <si>
+    <t>C207BC</t>
+  </si>
+  <si>
+    <t>Color</t>
+  </si>
+  <si>
+    <t>yellow</t>
+  </si>
+  <si>
+    <t>black</t>
+  </si>
+  <si>
+    <t>gray</t>
+  </si>
+  <si>
+    <t>red</t>
+  </si>
+  <si>
+    <t>purple</t>
+  </si>
+  <si>
+    <t>Geely Emgrand 7</t>
+  </si>
+  <si>
+    <t>Lexus ES</t>
+  </si>
+  <si>
+    <t>Mercedes-Benz S</t>
+  </si>
+  <si>
+    <t>Porsche 911 Cabriolet</t>
+  </si>
+  <si>
+    <t>Lamborghini Aventador</t>
   </si>
 </sst>
 </file>
@@ -1065,7 +1132,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1087,7 +1154,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -1390,10 +1456,12 @@
   <cols>
     <col min="1" max="1" width="8.109375" customWidth="1"/>
     <col min="2" max="2" width="9.5546875" customWidth="1"/>
-    <col min="4" max="4" width="13.21875" customWidth="1"/>
+    <col min="3" max="3" width="6.6640625" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" customWidth="1"/>
     <col min="5" max="5" width="9.33203125" customWidth="1"/>
     <col min="6" max="6" width="11.109375" customWidth="1"/>
     <col min="7" max="7" width="12" customWidth="1"/>
+    <col min="8" max="8" width="6.109375" customWidth="1"/>
     <col min="9" max="9" width="10.21875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2574,7 +2642,7 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
@@ -2593,17 +2661,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -2632,17 +2690,17 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -2671,17 +2729,17 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -2710,17 +2768,17 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -2749,17 +2807,17 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -2788,17 +2846,17 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -2827,17 +2885,17 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -2866,17 +2924,17 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -2905,17 +2963,17 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -2944,17 +3002,17 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -2970,8 +3028,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
+    <col min="3" max="3" width="6.6640625" customWidth="1"/>
     <col min="4" max="4" width="11.33203125" customWidth="1"/>
-    <col min="7" max="7" width="12" customWidth="1"/>
+    <col min="5" max="5" width="8.88671875" customWidth="1"/>
+    <col min="7" max="7" width="10" customWidth="1"/>
+    <col min="8" max="8" width="6.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -3020,7 +3081,7 @@
         <v>175263</v>
       </c>
       <c r="G2">
-        <v>89142961585</v>
+        <v>333223827</v>
       </c>
       <c r="H2">
         <v>1</v>
@@ -3046,7 +3107,7 @@
         <v>227427</v>
       </c>
       <c r="G3">
-        <v>89401049510</v>
+        <v>333223322</v>
       </c>
       <c r="H3">
         <v>3</v>
@@ -3072,7 +3133,7 @@
         <v>639159</v>
       </c>
       <c r="G4">
-        <v>89272640214</v>
+        <v>333225555</v>
       </c>
       <c r="H4">
         <v>4</v>
@@ -3098,7 +3159,7 @@
         <v>252425</v>
       </c>
       <c r="G5">
-        <v>89192484803</v>
+        <v>333221234</v>
       </c>
       <c r="H5">
         <v>5</v>
@@ -3124,7 +3185,7 @@
         <v>674539</v>
       </c>
       <c r="G6">
-        <v>89701705638</v>
+        <v>333227531</v>
       </c>
       <c r="H6">
         <v>5</v>
@@ -3150,7 +3211,7 @@
         <v>810879</v>
       </c>
       <c r="G7">
-        <v>89451314539</v>
+        <v>333220011</v>
       </c>
       <c r="H7">
         <v>4</v>
@@ -3182,17 +3243,17 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -3221,17 +3282,17 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -3241,7 +3302,7 @@
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
@@ -3260,22 +3321,17 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -3304,22 +3360,22 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -3328,6 +3384,50 @@
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView showRuler="0" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C4"/>
   <sheetViews>
@@ -3366,7 +3466,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -3400,7 +3500,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C4"/>
   <sheetViews>
@@ -3432,40 +3532,6 @@
     <row r="4" spans="1:3">
       <c r="A4">
         <v>63</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
-  <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3">
-        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -3494,12 +3560,12 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -3509,7 +3575,7 @@
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
@@ -3528,7 +3594,12 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2">
-        <v>68</v>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -3540,7 +3611,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N78"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A56" sqref="A56"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
@@ -5383,7 +5456,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
 </file>
 
@@ -5408,7 +5480,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -5437,7 +5509,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -5466,7 +5538,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -5495,7 +5567,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -5524,7 +5596,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -5553,7 +5625,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -5582,7 +5654,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -5591,6 +5663,35 @@
 </file>
 
 <file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView showRuler="0" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>75</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -5617,30 +5718,6 @@
     <row r="3" spans="1:3">
       <c r="A3">
         <v>77</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -5674,42 +5751,14 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>271</v>
-      </c>
-      <c r="C2" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -5906,13 +5955,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
@@ -5927,20 +5974,414 @@
         <v>101</v>
       </c>
     </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>274</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>275</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView showRuler="0" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
     <row r="2" spans="1:3">
       <c r="A2">
-        <v>3</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>269</v>
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>271</v>
       </c>
       <c r="C2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>287</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>276</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2">
         <v>4</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>288</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>277</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2">
+        <v>3</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>289</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>278</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2">
+        <v>29</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>290</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>279</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2">
+        <v>53</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>291</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>280</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -5949,6 +6390,46 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView showRuler="0" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>269</v>
+      </c>
+      <c r="C2" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C5"/>
   <sheetViews>
@@ -5985,35 +6466,6 @@
     <row r="5" spans="1:3">
       <c r="A5">
         <v>8</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2">
-        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -6042,7 +6494,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -6071,7 +6523,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ADD: Order writes to database ADD: Order has status ADD: Driver can see orders
</commit_message>
<xml_diff>
--- a/build-PSS_HomeWork4-Desktop_Qt_5_12_5_MinGW_64_bit-Release/release/DataBase/Accounts.xlsx
+++ b/build-PSS_HomeWork4-Desktop_Qt_5_12_5_MinGW_64_bit-Release/release/DataBase/Accounts.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Passenger" sheetId="1" r:id="rId1"/>
     <sheet name="Driver" sheetId="2" r:id="rId2"/>
     <sheet name="Orders" sheetId="47" r:id="rId3"/>
-    <sheet name="Activ orders" sheetId="54" r:id="rId4"/>
+    <sheet name="Active orders" sheetId="54" r:id="rId4"/>
     <sheet name="89959280771" sheetId="3" r:id="rId5"/>
     <sheet name="89180884879" sheetId="4" r:id="rId6"/>
     <sheet name="89962840843" sheetId="5" r:id="rId7"/>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="297">
   <si>
     <t>James</t>
   </si>
@@ -961,11 +961,30 @@
   <si>
     <t>Lamborghini Aventador</t>
   </si>
+  <si>
+    <t>LastOrderNumber</t>
+  </si>
+  <si>
+    <t>Universitetskay 1, k 3</t>
+  </si>
+  <si>
+    <t>Sportivnaya, 112</t>
+  </si>
+  <si>
+    <t>Pyaterochka</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="hh:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
+  </numFmts>
   <fonts count="6">
     <font>
       <sz val="11"/>
@@ -1011,7 +1030,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1027,6 +1046,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1132,7 +1157,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1153,7 +1178,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -3611,9 +3641,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N78"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A56" sqref="A56"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
@@ -5751,14 +5779,72 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
-  <sheetData/>
+  <cols>
+    <col min="7" max="7" width="10.33203125" customWidth="1"/>
+    <col min="8" max="8" width="6" customWidth="1"/>
+    <col min="9" max="9" width="15.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="H1" s="14" t="s">
+        <v>296</v>
+      </c>
+      <c r="I1" s="14" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="F2" s="15"/>
+      <c r="G2" s="16"/>
+      <c r="I2">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="F3" s="15"/>
+      <c r="G3" s="17"/>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="F4" s="15"/>
+      <c r="G4" s="17"/>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="F5" s="15"/>
+      <c r="G5" s="17"/>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="F6" s="15"/>
+      <c r="G6" s="17"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -5983,9 +6069,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
-    </sheetView>
+    <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
@@ -6016,10 +6100,10 @@
       <c r="C2">
         <v>0</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" t="s">
         <v>275</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" t="s">
         <v>282</v>
       </c>
     </row>
@@ -6040,19 +6124,21 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="8" max="8" width="6" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:8">
       <c r="A1" s="4" t="s">
         <v>99</v>
       </c>
@@ -6062,8 +6148,11 @@
       <c r="C1" s="4" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="H1" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2">
         <v>1</v>
       </c>
@@ -6074,9 +6163,20 @@
         <v>268</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:8">
       <c r="A3">
         <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="B4" t="s">
+        <v>294</v>
+      </c>
+      <c r="C4" t="s">
+        <v>295</v>
       </c>
     </row>
   </sheetData>
@@ -6088,9 +6188,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
+    <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
@@ -6115,16 +6213,16 @@
       <c r="A2">
         <v>2</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" t="s">
         <v>287</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" t="s">
         <v>276</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" t="s">
         <v>283</v>
       </c>
     </row>
@@ -6152,9 +6250,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
+    <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
@@ -6179,16 +6275,16 @@
       <c r="A2">
         <v>4</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" t="s">
         <v>288</v>
       </c>
       <c r="C2">
         <v>2</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" t="s">
         <v>277</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" t="s">
         <v>284</v>
       </c>
     </row>
@@ -6211,9 +6307,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
+    <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
@@ -6238,16 +6332,16 @@
       <c r="A2">
         <v>3</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" t="s">
         <v>289</v>
       </c>
       <c r="C2">
         <v>3</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" t="s">
         <v>278</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" t="s">
         <v>285</v>
       </c>
     </row>
@@ -6275,9 +6369,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
+    <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
@@ -6302,16 +6394,16 @@
       <c r="A2">
         <v>29</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" t="s">
         <v>290</v>
       </c>
       <c r="C2">
         <v>2</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" t="s">
         <v>279</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" t="s">
         <v>283</v>
       </c>
     </row>
@@ -6334,9 +6426,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
+    <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
@@ -6361,16 +6451,16 @@
       <c r="A2">
         <v>53</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" t="s">
         <v>291</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" t="s">
         <v>280</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" t="s">
         <v>286</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix bug with close order
</commit_message>
<xml_diff>
--- a/build-PSS_HomeWork4-Desktop_Qt_5_12_5_MinGW_64_bit-Release/release/DataBase/Accounts.xlsx
+++ b/build-PSS_HomeWork4-Desktop_Qt_5_12_5_MinGW_64_bit-Release/release/DataBase/Accounts.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9624" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Passenger" sheetId="1" r:id="rId1"/>
     <sheet name="Driver" sheetId="2" r:id="rId2"/>
     <sheet name="Orders" sheetId="47" r:id="rId3"/>
-    <sheet name="Active orders" sheetId="54" r:id="rId4"/>
+    <sheet name="Active_orders" sheetId="54" r:id="rId4"/>
     <sheet name="89959280771" sheetId="3" r:id="rId5"/>
     <sheet name="89180884879" sheetId="4" r:id="rId6"/>
     <sheet name="89962840843" sheetId="5" r:id="rId7"/>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="298">
   <si>
     <t>Leroy</t>
   </si>
@@ -888,6 +888,96 @@
       </rPr>
       <t/>
     </r>
+  </si>
+  <si>
+    <t>5023 Stamm Prairie Apt. 892 South Kali, DC 94246</t>
+  </si>
+  <si>
+    <t>89424 Connelly Inlet Suite 803 Bernardfort, MA 45891</t>
+  </si>
+  <si>
+    <t>12494 Hackett Heights West Marcofort, TN 31126-6622</t>
+  </si>
+  <si>
+    <t>97382 Liana Alley New Layla, NM 51451</t>
+  </si>
+  <si>
+    <t>497 Rutherford Summit West Marleehaven, TN 36706</t>
+  </si>
+  <si>
+    <t>742 Weissnat Crest Port Aishaborough, MN 67786</t>
+  </si>
+  <si>
+    <t>256 Breana Manors Apt. 530 Lake Milesmouth, WY 93121-8835</t>
+  </si>
+  <si>
+    <t>60682 Name Ville West Shannafort, ME 84411</t>
+  </si>
+  <si>
+    <t>43768 Duncan Trail Apt. 287 South Brock, WI 70383</t>
+  </si>
+  <si>
+    <t>30041 Satterfield Rapid Suite 472 Port Terrillbury, HI 63846-9856</t>
+  </si>
+  <si>
+    <t>99070 Stracke Roads East Karineland, HI 75112-3422</t>
+  </si>
+  <si>
+    <t>46243 Boyer Walks East Lukas, SC 15807-3842</t>
+  </si>
+  <si>
+    <t>538 Ondricka Crossing Skilesbury, MA 45237</t>
+  </si>
+  <si>
+    <t>I got too lazy to generate the addresses further.</t>
+  </si>
+  <si>
+    <t>46244 Boyer Walks East Lukas, SC 15807-3842</t>
+  </si>
+  <si>
+    <t>539 Ondricka Crossing Skilesbury, MA 45237</t>
+  </si>
+  <si>
+    <t>46245 Boyer Walks East Lukas, SC 15807-3842</t>
+  </si>
+  <si>
+    <t>540 Ondricka Crossing Skilesbury, MA 45237</t>
+  </si>
+  <si>
+    <t>46246 Boyer Walks East Lukas, SC 15807-3842</t>
+  </si>
+  <si>
+    <t>541 Ondricka Crossing Skilesbury, MA 45237</t>
+  </si>
+  <si>
+    <t>46247 Boyer Walks East Lukas, SC 15807-3842</t>
+  </si>
+  <si>
+    <t>542 Ondricka Crossing Skilesbury, MA 45237</t>
+  </si>
+  <si>
+    <t>46248 Boyer Walks East Lukas, SC 15807-3842</t>
+  </si>
+  <si>
+    <t>543 Ondricka Crossing Skilesbury, MA 45237</t>
+  </si>
+  <si>
+    <t>46249 Boyer Walks East Lukas, SC 15807-3842</t>
+  </si>
+  <si>
+    <t>544 Ondricka Crossing Skilesbury, MA 45237</t>
+  </si>
+  <si>
+    <t>46250 Boyer Walks East Lukas, SC 15807-3842</t>
+  </si>
+  <si>
+    <t>545 Ondricka Crossing Skilesbury, MA 45237</t>
+  </si>
+  <si>
+    <t>46251 Boyer Walks East Lukas, SC 15807-3842</t>
+  </si>
+  <si>
+    <t>546 Ondricka Crossing Skilesbury, MA 45237</t>
   </si>
 </sst>
 </file>
@@ -1070,7 +1160,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1095,6 +1185,7 @@
       <alignment horizontal="left" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -1392,7 +1483,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A25" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
@@ -3551,10 +3642,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N79"/>
+  <dimension ref="A1:N80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="K78" sqref="K78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3611,11 +3702,26 @@
       </c>
     </row>
     <row r="2" spans="1:14">
-      <c r="A2" s="12"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="2"/>
-      <c r="J2">
-        <v>78</v>
+      <c r="A2" s="12">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>268</v>
+      </c>
+      <c r="C2" t="s">
+        <v>269</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>80</v>
+      </c>
+      <c r="F2" s="11">
+        <v>0.63888888888888895</v>
+      </c>
+      <c r="G2" s="2">
+        <v>44180</v>
       </c>
       <c r="K2" s="8">
         <v>0</v>
@@ -3631,75 +3737,329 @@
       </c>
     </row>
     <row r="3" spans="1:14">
-      <c r="A3" s="12"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="2"/>
+      <c r="A3" s="12">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>270</v>
+      </c>
+      <c r="C3" t="s">
+        <v>271</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>158</v>
+      </c>
+      <c r="F3" s="11">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="G3" s="2">
+        <v>37305</v>
+      </c>
     </row>
     <row r="4" spans="1:14">
-      <c r="A4" s="12"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="2"/>
+      <c r="A4" s="12">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>272</v>
+      </c>
+      <c r="C4" t="s">
+        <v>273</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <v>239</v>
+      </c>
+      <c r="F4" s="11">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="G4" s="2">
+        <v>43907</v>
+      </c>
     </row>
     <row r="5" spans="1:14">
-      <c r="A5" s="12"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="2"/>
+      <c r="A5" s="12">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>274</v>
+      </c>
+      <c r="C5" t="s">
+        <v>273</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <v>304</v>
+      </c>
+      <c r="F5" s="11">
+        <v>0.78125</v>
+      </c>
+      <c r="G5" s="2">
+        <v>44180</v>
+      </c>
     </row>
     <row r="6" spans="1:14">
-      <c r="A6" s="12"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="2"/>
+      <c r="A6" s="12">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>275</v>
+      </c>
+      <c r="C6" t="s">
+        <v>276</v>
+      </c>
+      <c r="D6">
+        <v>3</v>
+      </c>
+      <c r="E6">
+        <v>317</v>
+      </c>
+      <c r="F6" s="11">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="G6" s="2">
+        <v>43887</v>
+      </c>
     </row>
     <row r="7" spans="1:14">
-      <c r="A7" s="12"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="2"/>
+      <c r="A7" s="12">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>277</v>
+      </c>
+      <c r="C7" t="s">
+        <v>278</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <v>204</v>
+      </c>
+      <c r="F7" s="11">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="G7" s="2">
+        <v>43868</v>
+      </c>
     </row>
     <row r="8" spans="1:14">
-      <c r="A8" s="12"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="13"/>
+      <c r="A8" s="12">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>279</v>
+      </c>
+      <c r="C8" t="s">
+        <v>280</v>
+      </c>
+      <c r="D8">
+        <v>3</v>
+      </c>
+      <c r="E8">
+        <v>142</v>
+      </c>
+      <c r="F8" s="11">
+        <v>0.47222222222222227</v>
+      </c>
+      <c r="G8" s="2">
+        <v>44169</v>
+      </c>
+      <c r="H8" s="13" t="s">
+        <v>281</v>
+      </c>
     </row>
     <row r="9" spans="1:14">
-      <c r="A9" s="12"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="2"/>
+      <c r="A9" s="12">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>282</v>
+      </c>
+      <c r="C9" t="s">
+        <v>283</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>306</v>
+      </c>
+      <c r="F9" s="11">
+        <v>0.51388888888888895</v>
+      </c>
+      <c r="G9" s="2">
+        <v>44170</v>
+      </c>
     </row>
     <row r="10" spans="1:14">
-      <c r="A10" s="12"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="2"/>
+      <c r="A10" s="12">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>284</v>
+      </c>
+      <c r="C10" t="s">
+        <v>285</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>270</v>
+      </c>
+      <c r="F10" s="11">
+        <v>0.55555555555555602</v>
+      </c>
+      <c r="G10" s="2">
+        <v>44171</v>
+      </c>
     </row>
     <row r="11" spans="1:14">
-      <c r="A11" s="12"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="2"/>
+      <c r="A11" s="12">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>286</v>
+      </c>
+      <c r="C11" t="s">
+        <v>287</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>96</v>
+      </c>
+      <c r="F11" s="11">
+        <v>0.59722222222222199</v>
+      </c>
+      <c r="G11" s="2">
+        <v>44172</v>
+      </c>
     </row>
     <row r="12" spans="1:14">
-      <c r="A12" s="12"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="2"/>
+      <c r="A12" s="12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>288</v>
+      </c>
+      <c r="C12" t="s">
+        <v>289</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>371</v>
+      </c>
+      <c r="F12" s="11">
+        <v>0.63888888888888895</v>
+      </c>
+      <c r="G12" s="2">
+        <v>44173</v>
+      </c>
     </row>
     <row r="13" spans="1:14">
-      <c r="A13" s="12"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="2"/>
+      <c r="A13" s="12">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>290</v>
+      </c>
+      <c r="C13" t="s">
+        <v>291</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+      <c r="E13">
+        <v>229</v>
+      </c>
+      <c r="F13" s="11">
+        <v>0.68055555555555602</v>
+      </c>
+      <c r="G13" s="2">
+        <v>44174</v>
+      </c>
     </row>
     <row r="14" spans="1:14">
-      <c r="A14" s="12"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="2"/>
+      <c r="A14" s="12">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>292</v>
+      </c>
+      <c r="C14" t="s">
+        <v>293</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>209</v>
+      </c>
+      <c r="F14" s="11">
+        <v>0.72222222222222199</v>
+      </c>
+      <c r="G14" s="2">
+        <v>44175</v>
+      </c>
     </row>
     <row r="15" spans="1:14">
-      <c r="A15" s="12"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="2"/>
+      <c r="A15" s="12">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>294</v>
+      </c>
+      <c r="C15" t="s">
+        <v>295</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>311</v>
+      </c>
+      <c r="F15" s="11">
+        <v>0.76388888888888895</v>
+      </c>
+      <c r="G15" s="2">
+        <v>44176</v>
+      </c>
     </row>
     <row r="16" spans="1:14">
-      <c r="A16" s="12"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="2"/>
+      <c r="A16" s="12">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>296</v>
+      </c>
+      <c r="C16" t="s">
+        <v>297</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>290</v>
+      </c>
+      <c r="F16" s="11">
+        <v>0.80555555555555602</v>
+      </c>
+      <c r="G16" s="2">
+        <v>44177</v>
+      </c>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="12">
@@ -5128,8 +5488,8 @@
       </c>
     </row>
     <row r="79" spans="1:7">
-      <c r="A79">
-        <v>79</v>
+      <c r="A79" s="12">
+        <v>78</v>
       </c>
       <c r="B79" t="s">
         <v>237</v>
@@ -5141,14 +5501,18 @@
         <v>3</v>
       </c>
       <c r="E79">
-        <v>342</v>
+        <v>403</v>
       </c>
       <c r="F79" s="15">
-        <v>2.9166666666666698E-2</v>
-      </c>
-      <c r="G79" s="16">
+        <v>7.1527777777777801E-2</v>
+      </c>
+      <c r="G79" s="17">
         <v>44312</v>
       </c>
+    </row>
+    <row r="80" spans="1:7">
+      <c r="F80" s="15"/>
+      <c r="G80" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5450,7 +5814,7 @@
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -5498,7 +5862,7 @@
       <c r="F2" s="15"/>
       <c r="G2" s="16"/>
       <c r="J2">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -5842,6 +6206,9 @@
       </c>
     </row>
     <row r="4" spans="1:3">
+      <c r="A4">
+        <v>78</v>
+      </c>
       <c r="B4" t="s">
         <v>260</v>
       </c>
@@ -5975,7 +6342,7 @@
 
 <file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
@@ -6028,6 +6395,11 @@
     <row r="5" spans="1:5">
       <c r="A5">
         <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6">
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix: bug with orders
</commit_message>
<xml_diff>
--- a/build-PSS_HomeWork4-Desktop_Qt_5_12_5_MinGW_64_bit-Release/release/DataBase/Accounts.xlsx
+++ b/build-PSS_HomeWork4-Desktop_Qt_5_12_5_MinGW_64_bit-Release/release/DataBase/Accounts.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9624" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="51"/>
   </bookViews>
   <sheets>
     <sheet name="Passenger" sheetId="1" r:id="rId1"/>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="301">
   <si>
     <t>Leroy</t>
   </si>
@@ -979,45 +979,55 @@
   <si>
     <t>546 Ondricka Crossing Skilesbury, MA 45237</t>
   </si>
+  <si>
+    <t>st. Raisoveta, 8</t>
+  </si>
+  <si>
+    <t>89959280771</t>
+  </si>
+  <si>
+    <t/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="hh:mm:ss"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="176" formatCode="yyyy-mm-dd"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <charset val="204"/>
       <family val="2"/>
-      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF800080"/>
       <name val="Arial Unicode MS"/>
+      <charset val="204"/>
       <family val="2"/>
-      <charset val="204"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FFC0C0C0"/>
       <name val="Arial Unicode MS"/>
+      <charset val="204"/>
       <family val="2"/>
-      <charset val="204"/>
     </font>
     <font>
       <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <charset val="204"/>
       <family val="2"/>
-      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1031,6 +1041,9 @@
       <color rgb="FFC0C0C0"/>
       <name val="Arial Unicode MS"/>
       <family val="2"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="5">
@@ -1160,7 +1173,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1186,10 +1199,11 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1483,9 +1497,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="8.109375" customWidth="1"/>
     <col min="2" max="2" width="9.5546875" customWidth="1"/>
@@ -1498,7 +1512,7 @@
     <col min="9" max="9" width="10.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1">
       <c r="A1" s="3" t="s">
         <v>87</v>
       </c>
@@ -1524,7 +1538,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2">
       <c r="A2" t="s">
         <v>262</v>
       </c>
@@ -1534,7 +1548,7 @@
       <c r="C2" t="s">
         <v>90</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="2" t="n">
         <v>23864</v>
       </c>
       <c r="E2">
@@ -1550,7 +1564,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -1560,7 +1574,7 @@
       <c r="C3" t="s">
         <v>90</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="2" t="n">
         <v>26467</v>
       </c>
       <c r="E3">
@@ -1576,7 +1590,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -1586,7 +1600,7 @@
       <c r="C4" t="s">
         <v>90</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="2" t="n">
         <v>31167</v>
       </c>
       <c r="E4">
@@ -1602,7 +1616,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -1612,7 +1626,7 @@
       <c r="C5" t="s">
         <v>90</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="2" t="n">
         <v>32852</v>
       </c>
       <c r="E5">
@@ -1628,7 +1642,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -1638,7 +1652,7 @@
       <c r="C6" t="s">
         <v>90</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="2" t="n">
         <v>26494</v>
       </c>
       <c r="E6">
@@ -1654,7 +1668,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -1664,7 +1678,7 @@
       <c r="C7" t="s">
         <v>91</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="2" t="n">
         <v>33284</v>
       </c>
       <c r="E7">
@@ -1680,7 +1694,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -1690,7 +1704,7 @@
       <c r="C8" t="s">
         <v>91</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="2" t="n">
         <v>27334</v>
       </c>
       <c r="E8">
@@ -1706,7 +1720,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -1716,7 +1730,7 @@
       <c r="C9" t="s">
         <v>90</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="2" t="n">
         <v>37211</v>
       </c>
       <c r="E9">
@@ -1732,7 +1746,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -1742,7 +1756,7 @@
       <c r="C10" t="s">
         <v>90</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="2" t="n">
         <v>28951</v>
       </c>
       <c r="E10">
@@ -1758,7 +1772,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -1768,7 +1782,7 @@
       <c r="C11" t="s">
         <v>90</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="2" t="n">
         <v>30962</v>
       </c>
       <c r="E11">
@@ -1784,7 +1798,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -1794,7 +1808,7 @@
       <c r="C12" t="s">
         <v>91</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12" s="2" t="n">
         <v>37478</v>
       </c>
       <c r="E12">
@@ -1810,7 +1824,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -1820,7 +1834,7 @@
       <c r="C13" t="s">
         <v>91</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D13" s="2" t="n">
         <v>35118</v>
       </c>
       <c r="E13">
@@ -1836,7 +1850,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14">
       <c r="A14" t="s">
         <v>1</v>
       </c>
@@ -1846,7 +1860,7 @@
       <c r="C14" t="s">
         <v>90</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D14" s="2" t="n">
         <v>24495</v>
       </c>
       <c r="E14">
@@ -1862,7 +1876,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15">
       <c r="A15" t="s">
         <v>10</v>
       </c>
@@ -1872,7 +1886,7 @@
       <c r="C15" t="s">
         <v>90</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D15" s="2" t="n">
         <v>27707</v>
       </c>
       <c r="E15">
@@ -1888,7 +1902,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16">
       <c r="A16" t="s">
         <v>11</v>
       </c>
@@ -1898,7 +1912,7 @@
       <c r="C16" t="s">
         <v>90</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16" s="2" t="n">
         <v>34909</v>
       </c>
       <c r="E16">
@@ -1924,7 +1938,7 @@
       <c r="C17" t="s">
         <v>90</v>
       </c>
-      <c r="D17" s="2">
+      <c r="D17" s="2" t="n">
         <v>27606</v>
       </c>
       <c r="E17">
@@ -1950,7 +1964,7 @@
       <c r="C18" t="s">
         <v>90</v>
       </c>
-      <c r="D18" s="2">
+      <c r="D18" s="2" t="n">
         <v>26204</v>
       </c>
       <c r="E18">
@@ -1976,7 +1990,7 @@
       <c r="C19" t="s">
         <v>90</v>
       </c>
-      <c r="D19" s="2">
+      <c r="D19" s="2" t="n">
         <v>24456</v>
       </c>
       <c r="E19">
@@ -2002,7 +2016,7 @@
       <c r="C20" t="s">
         <v>91</v>
       </c>
-      <c r="D20" s="2">
+      <c r="D20" s="2" t="n">
         <v>25617</v>
       </c>
       <c r="E20">
@@ -2028,7 +2042,7 @@
       <c r="C21" t="s">
         <v>90</v>
       </c>
-      <c r="D21" s="2">
+      <c r="D21" s="2" t="n">
         <v>30392</v>
       </c>
       <c r="E21">
@@ -2054,7 +2068,7 @@
       <c r="C22" t="s">
         <v>91</v>
       </c>
-      <c r="D22" s="2">
+      <c r="D22" s="2" t="n">
         <v>34683</v>
       </c>
       <c r="E22">
@@ -2080,7 +2094,7 @@
       <c r="C23" t="s">
         <v>91</v>
       </c>
-      <c r="D23" s="2">
+      <c r="D23" s="2" t="n">
         <v>29643</v>
       </c>
       <c r="E23">
@@ -2106,7 +2120,7 @@
       <c r="C24" t="s">
         <v>91</v>
       </c>
-      <c r="D24" s="2">
+      <c r="D24" s="2" t="n">
         <v>33276</v>
       </c>
       <c r="E24">
@@ -2132,7 +2146,7 @@
       <c r="C25" t="s">
         <v>90</v>
       </c>
-      <c r="D25" s="2">
+      <c r="D25" s="2" t="n">
         <v>27002</v>
       </c>
       <c r="E25">
@@ -2158,7 +2172,7 @@
       <c r="C26" t="s">
         <v>91</v>
       </c>
-      <c r="D26" s="2">
+      <c r="D26" s="2" t="n">
         <v>36440</v>
       </c>
       <c r="E26">
@@ -2184,7 +2198,7 @@
       <c r="C27" t="s">
         <v>90</v>
       </c>
-      <c r="D27" s="2">
+      <c r="D27" s="2" t="n">
         <v>26848</v>
       </c>
       <c r="E27">
@@ -2210,7 +2224,7 @@
       <c r="C28" t="s">
         <v>91</v>
       </c>
-      <c r="D28" s="2">
+      <c r="D28" s="2" t="n">
         <v>36235</v>
       </c>
       <c r="E28">
@@ -2236,7 +2250,7 @@
       <c r="C29" t="s">
         <v>90</v>
       </c>
-      <c r="D29" s="2">
+      <c r="D29" s="2" t="n">
         <v>27142</v>
       </c>
       <c r="E29">
@@ -2262,7 +2276,7 @@
       <c r="C30" t="s">
         <v>91</v>
       </c>
-      <c r="D30" s="2">
+      <c r="D30" s="2" t="n">
         <v>22558</v>
       </c>
       <c r="E30">
@@ -2288,7 +2302,7 @@
       <c r="C31" t="s">
         <v>90</v>
       </c>
-      <c r="D31" s="2">
+      <c r="D31" s="2" t="n">
         <v>31838</v>
       </c>
       <c r="E31">
@@ -2314,7 +2328,7 @@
       <c r="C32" t="s">
         <v>90</v>
       </c>
-      <c r="D32" s="2">
+      <c r="D32" s="2" t="n">
         <v>35991</v>
       </c>
       <c r="E32">
@@ -2340,7 +2354,7 @@
       <c r="C33" t="s">
         <v>90</v>
       </c>
-      <c r="D33" s="2">
+      <c r="D33" s="2" t="n">
         <v>29065</v>
       </c>
       <c r="E33">
@@ -2366,7 +2380,7 @@
       <c r="C34" t="s">
         <v>90</v>
       </c>
-      <c r="D34" s="2">
+      <c r="D34" s="2" t="n">
         <v>31282</v>
       </c>
       <c r="E34">
@@ -2392,7 +2406,7 @@
       <c r="C35" t="s">
         <v>91</v>
       </c>
-      <c r="D35" s="2">
+      <c r="D35" s="2" t="n">
         <v>22663</v>
       </c>
       <c r="E35">
@@ -2418,7 +2432,7 @@
       <c r="C36" t="s">
         <v>91</v>
       </c>
-      <c r="D36" s="2">
+      <c r="D36" s="2" t="n">
         <v>33782</v>
       </c>
       <c r="E36">
@@ -2444,7 +2458,7 @@
       <c r="C37" t="s">
         <v>90</v>
       </c>
-      <c r="D37" s="2">
+      <c r="D37" s="2" t="n">
         <v>34169</v>
       </c>
       <c r="E37">
@@ -2470,7 +2484,7 @@
       <c r="C38" t="s">
         <v>90</v>
       </c>
-      <c r="D38" s="2">
+      <c r="D38" s="2" t="n">
         <v>25868</v>
       </c>
       <c r="E38">
@@ -2496,7 +2510,7 @@
       <c r="C39" t="s">
         <v>90</v>
       </c>
-      <c r="D39" s="2">
+      <c r="D39" s="2" t="n">
         <v>27197</v>
       </c>
       <c r="E39">
@@ -2522,7 +2536,7 @@
       <c r="C40" t="s">
         <v>91</v>
       </c>
-      <c r="D40" s="2">
+      <c r="D40" s="2" t="n">
         <v>31031</v>
       </c>
       <c r="E40">
@@ -2548,7 +2562,7 @@
       <c r="C41" t="s">
         <v>91</v>
       </c>
-      <c r="D41" s="2">
+      <c r="D41" s="2" t="n">
         <v>24333</v>
       </c>
       <c r="E41">
@@ -2574,7 +2588,7 @@
       <c r="C42" t="s">
         <v>91</v>
       </c>
-      <c r="D42" s="2">
+      <c r="D42" s="2" t="n">
         <v>30275</v>
       </c>
       <c r="E42">
@@ -2600,7 +2614,7 @@
       <c r="C43" t="s">
         <v>90</v>
       </c>
-      <c r="D43" s="2">
+      <c r="D43" s="2" t="n">
         <v>29192</v>
       </c>
       <c r="E43">
@@ -2626,7 +2640,7 @@
       <c r="C44" t="s">
         <v>90</v>
       </c>
-      <c r="D44" s="2">
+      <c r="D44" s="2" t="n">
         <v>29973</v>
       </c>
       <c r="E44">
@@ -2652,7 +2666,7 @@
       <c r="C45" t="s">
         <v>90</v>
       </c>
-      <c r="D45" s="2">
+      <c r="D45" s="2" t="n">
         <v>31402</v>
       </c>
       <c r="E45">
@@ -2679,7 +2693,7 @@
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="4" t="s">
@@ -2708,7 +2722,7 @@
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="4" t="s">
@@ -2747,7 +2761,7 @@
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="4" t="s">
@@ -2786,7 +2800,7 @@
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="4" t="s">
@@ -2825,7 +2839,7 @@
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="4" t="s">
@@ -2864,7 +2878,7 @@
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="4" t="s">
@@ -2903,7 +2917,7 @@
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="4" t="s">
@@ -2942,7 +2956,7 @@
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="4" t="s">
@@ -2981,7 +2995,7 @@
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="4" t="s">
@@ -3020,7 +3034,7 @@
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="4" t="s">
@@ -3059,7 +3073,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="6.6640625" customWidth="1"/>
     <col min="4" max="4" width="11.33203125" customWidth="1"/>
@@ -3104,7 +3118,7 @@
       <c r="C2" t="s">
         <v>91</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="2" t="n">
         <v>35888</v>
       </c>
       <c r="E2">
@@ -3130,7 +3144,7 @@
       <c r="C3" t="s">
         <v>91</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="2" t="n">
         <v>26607</v>
       </c>
       <c r="E3">
@@ -3156,7 +3170,7 @@
       <c r="C4" t="s">
         <v>91</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="2" t="n">
         <v>36103</v>
       </c>
       <c r="E4">
@@ -3182,7 +3196,7 @@
       <c r="C5" t="s">
         <v>90</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="2" t="n">
         <v>32991</v>
       </c>
       <c r="E5">
@@ -3208,7 +3222,7 @@
       <c r="C6" t="s">
         <v>90</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="2" t="n">
         <v>35858</v>
       </c>
       <c r="E6">
@@ -3234,7 +3248,7 @@
       <c r="C7" t="s">
         <v>90</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="2" t="n">
         <v>24559</v>
       </c>
       <c r="E7">
@@ -3261,7 +3275,7 @@
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="4" t="s">
@@ -3300,7 +3314,7 @@
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="4" t="s">
@@ -3339,7 +3353,7 @@
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="4" t="s">
@@ -3378,7 +3392,7 @@
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="4" t="s">
@@ -3422,7 +3436,7 @@
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="4" t="s">
@@ -3466,7 +3480,7 @@
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="4" t="s">
@@ -3505,7 +3519,7 @@
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="4" t="s">
@@ -3539,7 +3553,7 @@
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="4" t="s">
@@ -3578,7 +3592,7 @@
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="4" t="s">
@@ -3612,7 +3626,7 @@
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="4" t="s">
@@ -3642,13 +3656,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N80"/>
+  <dimension ref="A1:N81"/>
   <sheetViews>
-    <sheetView topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="K78" sqref="K78"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12.33203125" customWidth="1"/>
     <col min="2" max="2" width="13.6640625" customWidth="1"/>
@@ -3663,7 +3675,7 @@
     <col min="13" max="13" width="11.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15">
+    <row r="1">
       <c r="A1" s="4" t="s">
         <v>109</v>
       </c>
@@ -3701,7 +3713,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2">
       <c r="A2" s="12">
         <v>1</v>
       </c>
@@ -3717,10 +3729,10 @@
       <c r="E2">
         <v>80</v>
       </c>
-      <c r="F2" s="11">
-        <v>0.63888888888888895</v>
-      </c>
-      <c r="G2" s="2">
+      <c r="F2" s="11" t="n">
+        <v>0.638888888888889</v>
+      </c>
+      <c r="G2" s="2" t="n">
         <v>44180</v>
       </c>
       <c r="K2" s="8">
@@ -3736,7 +3748,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3">
       <c r="A3" s="12">
         <v>2</v>
       </c>
@@ -3752,14 +3764,14 @@
       <c r="E3">
         <v>158</v>
       </c>
-      <c r="F3" s="11">
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="G3" s="2">
+      <c r="F3" s="11" t="n">
+        <v>0.6666666666666666</v>
+      </c>
+      <c r="G3" s="2" t="n">
         <v>37305</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4">
       <c r="A4" s="12">
         <v>3</v>
       </c>
@@ -3775,14 +3787,14 @@
       <c r="E4">
         <v>239</v>
       </c>
-      <c r="F4" s="11">
-        <v>0.39583333333333331</v>
-      </c>
-      <c r="G4" s="2">
+      <c r="F4" s="11" t="n">
+        <v>0.3958333333333333</v>
+      </c>
+      <c r="G4" s="2" t="n">
         <v>43907</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5">
       <c r="A5" s="12">
         <v>4</v>
       </c>
@@ -3798,14 +3810,14 @@
       <c r="E5">
         <v>304</v>
       </c>
-      <c r="F5" s="11">
+      <c r="F5" s="11" t="n">
         <v>0.78125</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5" s="2" t="n">
         <v>44180</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6">
       <c r="A6" s="12">
         <v>5</v>
       </c>
@@ -3821,14 +3833,14 @@
       <c r="E6">
         <v>317</v>
       </c>
-      <c r="F6" s="11">
-        <v>0.79166666666666663</v>
-      </c>
-      <c r="G6" s="2">
+      <c r="F6" s="11" t="n">
+        <v>0.7916666666666666</v>
+      </c>
+      <c r="G6" s="2" t="n">
         <v>43887</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7">
       <c r="A7" s="12">
         <v>6</v>
       </c>
@@ -3844,14 +3856,14 @@
       <c r="E7">
         <v>204</v>
       </c>
-      <c r="F7" s="11">
-        <v>0.91666666666666663</v>
-      </c>
-      <c r="G7" s="2">
+      <c r="F7" s="11" t="n">
+        <v>0.9166666666666666</v>
+      </c>
+      <c r="G7" s="2" t="n">
         <v>43868</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8">
       <c r="A8" s="12">
         <v>7</v>
       </c>
@@ -3867,17 +3879,17 @@
       <c r="E8">
         <v>142</v>
       </c>
-      <c r="F8" s="11">
+      <c r="F8" s="11" t="n">
         <v>0.47222222222222227</v>
       </c>
-      <c r="G8" s="2">
+      <c r="G8" s="2" t="n">
         <v>44169</v>
       </c>
       <c r="H8" s="13" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9">
       <c r="A9" s="12">
         <v>8</v>
       </c>
@@ -3893,14 +3905,14 @@
       <c r="E9">
         <v>306</v>
       </c>
-      <c r="F9" s="11">
-        <v>0.51388888888888895</v>
-      </c>
-      <c r="G9" s="2">
+      <c r="F9" s="11" t="n">
+        <v>0.513888888888889</v>
+      </c>
+      <c r="G9" s="2" t="n">
         <v>44170</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10">
       <c r="A10" s="12">
         <v>9</v>
       </c>
@@ -3916,14 +3928,14 @@
       <c r="E10">
         <v>270</v>
       </c>
-      <c r="F10" s="11">
-        <v>0.55555555555555602</v>
-      </c>
-      <c r="G10" s="2">
+      <c r="F10" s="11" t="n">
+        <v>0.555555555555556</v>
+      </c>
+      <c r="G10" s="2" t="n">
         <v>44171</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11">
       <c r="A11" s="12">
         <v>10</v>
       </c>
@@ -3939,14 +3951,14 @@
       <c r="E11">
         <v>96</v>
       </c>
-      <c r="F11" s="11">
-        <v>0.59722222222222199</v>
-      </c>
-      <c r="G11" s="2">
+      <c r="F11" s="11" t="n">
+        <v>0.597222222222222</v>
+      </c>
+      <c r="G11" s="2" t="n">
         <v>44172</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12">
       <c r="A12" s="12">
         <v>11</v>
       </c>
@@ -3962,14 +3974,14 @@
       <c r="E12">
         <v>371</v>
       </c>
-      <c r="F12" s="11">
-        <v>0.63888888888888895</v>
-      </c>
-      <c r="G12" s="2">
+      <c r="F12" s="11" t="n">
+        <v>0.638888888888889</v>
+      </c>
+      <c r="G12" s="2" t="n">
         <v>44173</v>
       </c>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13">
       <c r="A13" s="12">
         <v>12</v>
       </c>
@@ -3985,14 +3997,14 @@
       <c r="E13">
         <v>229</v>
       </c>
-      <c r="F13" s="11">
-        <v>0.68055555555555602</v>
-      </c>
-      <c r="G13" s="2">
+      <c r="F13" s="11" t="n">
+        <v>0.680555555555556</v>
+      </c>
+      <c r="G13" s="2" t="n">
         <v>44174</v>
       </c>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14">
       <c r="A14" s="12">
         <v>13</v>
       </c>
@@ -4008,14 +4020,14 @@
       <c r="E14">
         <v>209</v>
       </c>
-      <c r="F14" s="11">
-        <v>0.72222222222222199</v>
-      </c>
-      <c r="G14" s="2">
+      <c r="F14" s="11" t="n">
+        <v>0.722222222222222</v>
+      </c>
+      <c r="G14" s="2" t="n">
         <v>44175</v>
       </c>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15">
       <c r="A15" s="12">
         <v>14</v>
       </c>
@@ -4031,14 +4043,14 @@
       <c r="E15">
         <v>311</v>
       </c>
-      <c r="F15" s="11">
-        <v>0.76388888888888895</v>
-      </c>
-      <c r="G15" s="2">
+      <c r="F15" s="11" t="n">
+        <v>0.763888888888889</v>
+      </c>
+      <c r="G15" s="2" t="n">
         <v>44176</v>
       </c>
     </row>
-    <row r="16" spans="1:14">
+    <row r="16">
       <c r="A16" s="12">
         <v>15</v>
       </c>
@@ -4054,14 +4066,14 @@
       <c r="E16">
         <v>290</v>
       </c>
-      <c r="F16" s="11">
-        <v>0.80555555555555602</v>
-      </c>
-      <c r="G16" s="2">
+      <c r="F16" s="11" t="n">
+        <v>0.805555555555556</v>
+      </c>
+      <c r="G16" s="2" t="n">
         <v>44177</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:14">
       <c r="A17" s="12">
         <v>16</v>
       </c>
@@ -4077,14 +4089,14 @@
       <c r="E17">
         <v>141</v>
       </c>
-      <c r="F17" s="11">
-        <v>0.84722222222222199</v>
-      </c>
-      <c r="G17" s="2">
+      <c r="F17" s="11" t="n">
+        <v>0.847222222222222</v>
+      </c>
+      <c r="G17" s="2" t="n">
         <v>44178</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:14">
       <c r="A18" s="12">
         <v>17</v>
       </c>
@@ -4100,14 +4112,14 @@
       <c r="E18">
         <v>118</v>
       </c>
-      <c r="F18" s="11">
-        <v>0.88888888888888895</v>
-      </c>
-      <c r="G18" s="2">
+      <c r="F18" s="11" t="n">
+        <v>0.888888888888889</v>
+      </c>
+      <c r="G18" s="2" t="n">
         <v>44179</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:14">
       <c r="A19" s="12">
         <v>18</v>
       </c>
@@ -4123,14 +4135,14 @@
       <c r="E19">
         <v>192</v>
       </c>
-      <c r="F19" s="11">
-        <v>0.93055555555555602</v>
-      </c>
-      <c r="G19" s="2">
+      <c r="F19" s="11" t="n">
+        <v>0.930555555555556</v>
+      </c>
+      <c r="G19" s="2" t="n">
         <v>44180</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:14">
       <c r="A20" s="12">
         <v>19</v>
       </c>
@@ -4146,14 +4158,14 @@
       <c r="E20">
         <v>146</v>
       </c>
-      <c r="F20" s="11">
-        <v>0.97222222222222199</v>
-      </c>
-      <c r="G20" s="2">
+      <c r="F20" s="11" t="n">
+        <v>0.972222222222222</v>
+      </c>
+      <c r="G20" s="2" t="n">
         <v>44181</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:14">
       <c r="A21" s="12">
         <v>20</v>
       </c>
@@ -4169,14 +4181,14 @@
       <c r="E21">
         <v>284</v>
       </c>
-      <c r="F21" s="11">
-        <v>1.3888888888888888E-2</v>
-      </c>
-      <c r="G21" s="2">
+      <c r="F21" s="11" t="n">
+        <v>0.013888888888888888</v>
+      </c>
+      <c r="G21" s="2" t="n">
         <v>44182</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:14">
       <c r="A22" s="12">
         <v>21</v>
       </c>
@@ -4192,14 +4204,14 @@
       <c r="E22">
         <v>323</v>
       </c>
-      <c r="F22" s="11">
-        <v>5.5555555555555552E-2</v>
-      </c>
-      <c r="G22" s="2">
+      <c r="F22" s="11" t="n">
+        <v>0.05555555555555555</v>
+      </c>
+      <c r="G22" s="2" t="n">
         <v>44183</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:14">
       <c r="A23" s="12">
         <v>22</v>
       </c>
@@ -4215,14 +4227,14 @@
       <c r="E23">
         <v>118</v>
       </c>
-      <c r="F23" s="11">
-        <v>9.7222222222222224E-2</v>
-      </c>
-      <c r="G23" s="2">
+      <c r="F23" s="11" t="n">
+        <v>0.09722222222222222</v>
+      </c>
+      <c r="G23" s="2" t="n">
         <v>44184</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:14">
       <c r="A24" s="12">
         <v>23</v>
       </c>
@@ -4238,14 +4250,14 @@
       <c r="E24">
         <v>292</v>
       </c>
-      <c r="F24" s="11">
+      <c r="F24" s="11" t="n">
         <v>0.1388888888888889</v>
       </c>
-      <c r="G24" s="2">
+      <c r="G24" s="2" t="n">
         <v>44185</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:14">
       <c r="A25" s="12">
         <v>24</v>
       </c>
@@ -4261,14 +4273,14 @@
       <c r="E25">
         <v>218</v>
       </c>
-      <c r="F25" s="11">
+      <c r="F25" s="11" t="n">
         <v>0.18055555555555555</v>
       </c>
-      <c r="G25" s="2">
+      <c r="G25" s="2" t="n">
         <v>44186</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:14">
       <c r="A26" s="12">
         <v>25</v>
       </c>
@@ -4284,14 +4296,14 @@
       <c r="E26">
         <v>205</v>
       </c>
-      <c r="F26" s="11">
-        <v>0.22222222222222221</v>
-      </c>
-      <c r="G26" s="2">
+      <c r="F26" s="11" t="n">
+        <v>0.2222222222222222</v>
+      </c>
+      <c r="G26" s="2" t="n">
         <v>44187</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:14">
       <c r="A27" s="12">
         <v>26</v>
       </c>
@@ -4307,14 +4319,14 @@
       <c r="E27">
         <v>163</v>
       </c>
-      <c r="F27" s="11">
+      <c r="F27" s="11" t="n">
         <v>0.2638888888888889</v>
       </c>
-      <c r="G27" s="2">
+      <c r="G27" s="2" t="n">
         <v>44188</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:14">
       <c r="A28" s="12">
         <v>27</v>
       </c>
@@ -4330,14 +4342,14 @@
       <c r="E28">
         <v>196</v>
       </c>
-      <c r="F28" s="11">
-        <v>0.30555555555555552</v>
-      </c>
-      <c r="G28" s="2">
+      <c r="F28" s="11" t="n">
+        <v>0.3055555555555555</v>
+      </c>
+      <c r="G28" s="2" t="n">
         <v>44189</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:14">
       <c r="A29" s="12">
         <v>28</v>
       </c>
@@ -4353,14 +4365,14 @@
       <c r="E29">
         <v>223</v>
       </c>
-      <c r="F29" s="11">
+      <c r="F29" s="11" t="n">
         <v>0.34722222222222227</v>
       </c>
-      <c r="G29" s="2">
+      <c r="G29" s="2" t="n">
         <v>44190</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:14">
       <c r="A30" s="12">
         <v>29</v>
       </c>
@@ -4376,14 +4388,14 @@
       <c r="E30">
         <v>367</v>
       </c>
-      <c r="F30" s="11">
+      <c r="F30" s="11" t="n">
         <v>0.3888888888888889</v>
       </c>
-      <c r="G30" s="2">
+      <c r="G30" s="2" t="n">
         <v>44191</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:14">
       <c r="A31" s="12">
         <v>30</v>
       </c>
@@ -4399,14 +4411,14 @@
       <c r="E31">
         <v>330</v>
       </c>
-      <c r="F31" s="11">
-        <v>0.43055555555555558</v>
-      </c>
-      <c r="G31" s="2">
+      <c r="F31" s="11" t="n">
+        <v>0.4305555555555556</v>
+      </c>
+      <c r="G31" s="2" t="n">
         <v>44192</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:14">
       <c r="A32" s="12">
         <v>31</v>
       </c>
@@ -4422,10 +4434,10 @@
       <c r="E32">
         <v>181</v>
       </c>
-      <c r="F32" s="11">
+      <c r="F32" s="11" t="n">
         <v>0.47222222222222227</v>
       </c>
-      <c r="G32" s="2">
+      <c r="G32" s="2" t="n">
         <v>44193</v>
       </c>
     </row>
@@ -4445,10 +4457,10 @@
       <c r="E33">
         <v>184</v>
       </c>
-      <c r="F33" s="11">
-        <v>0.51388888888888895</v>
-      </c>
-      <c r="G33" s="2">
+      <c r="F33" s="11" t="n">
+        <v>0.513888888888889</v>
+      </c>
+      <c r="G33" s="2" t="n">
         <v>44194</v>
       </c>
     </row>
@@ -4468,10 +4480,10 @@
       <c r="E34">
         <v>245</v>
       </c>
-      <c r="F34" s="11">
-        <v>0.55555555555555558</v>
-      </c>
-      <c r="G34" s="2">
+      <c r="F34" s="11" t="n">
+        <v>0.5555555555555556</v>
+      </c>
+      <c r="G34" s="2" t="n">
         <v>44195</v>
       </c>
     </row>
@@ -4491,10 +4503,10 @@
       <c r="E35">
         <v>342</v>
       </c>
-      <c r="F35" s="11">
-        <v>0.59722222222222221</v>
-      </c>
-      <c r="G35" s="2">
+      <c r="F35" s="11" t="n">
+        <v>0.5972222222222222</v>
+      </c>
+      <c r="G35" s="2" t="n">
         <v>44196</v>
       </c>
     </row>
@@ -4514,10 +4526,10 @@
       <c r="E36">
         <v>306</v>
       </c>
-      <c r="F36" s="11">
-        <v>0.63888888888888895</v>
-      </c>
-      <c r="G36" s="2">
+      <c r="F36" s="11" t="n">
+        <v>0.638888888888889</v>
+      </c>
+      <c r="G36" s="2" t="n">
         <v>44197</v>
       </c>
     </row>
@@ -4537,10 +4549,10 @@
       <c r="E37">
         <v>190</v>
       </c>
-      <c r="F37" s="11">
-        <v>0.68055555555555547</v>
-      </c>
-      <c r="G37" s="2">
+      <c r="F37" s="11" t="n">
+        <v>0.6805555555555555</v>
+      </c>
+      <c r="G37" s="2" t="n">
         <v>44198</v>
       </c>
     </row>
@@ -4560,10 +4572,10 @@
       <c r="E38">
         <v>282</v>
       </c>
-      <c r="F38" s="11">
-        <v>0.72222222222222221</v>
-      </c>
-      <c r="G38" s="2">
+      <c r="F38" s="11" t="n">
+        <v>0.7222222222222222</v>
+      </c>
+      <c r="G38" s="2" t="n">
         <v>44199</v>
       </c>
     </row>
@@ -4583,10 +4595,10 @@
       <c r="E39">
         <v>232</v>
       </c>
-      <c r="F39" s="11">
-        <v>0.76388888888888884</v>
-      </c>
-      <c r="G39" s="2">
+      <c r="F39" s="11" t="n">
+        <v>0.7638888888888888</v>
+      </c>
+      <c r="G39" s="2" t="n">
         <v>44200</v>
       </c>
     </row>
@@ -4606,10 +4618,10 @@
       <c r="E40">
         <v>155</v>
       </c>
-      <c r="F40" s="11">
-        <v>0.80555555555555547</v>
-      </c>
-      <c r="G40" s="2">
+      <c r="F40" s="11" t="n">
+        <v>0.8055555555555555</v>
+      </c>
+      <c r="G40" s="2" t="n">
         <v>44201</v>
       </c>
     </row>
@@ -4629,10 +4641,10 @@
       <c r="E41">
         <v>320</v>
       </c>
-      <c r="F41" s="11">
-        <v>0.84722222222222221</v>
-      </c>
-      <c r="G41" s="2">
+      <c r="F41" s="11" t="n">
+        <v>0.8472222222222222</v>
+      </c>
+      <c r="G41" s="2" t="n">
         <v>44202</v>
       </c>
     </row>
@@ -4652,10 +4664,10 @@
       <c r="E42">
         <v>150</v>
       </c>
-      <c r="F42" s="11">
-        <v>0.88888888888888884</v>
-      </c>
-      <c r="G42" s="2">
+      <c r="F42" s="11" t="n">
+        <v>0.8888888888888888</v>
+      </c>
+      <c r="G42" s="2" t="n">
         <v>44203</v>
       </c>
     </row>
@@ -4675,10 +4687,10 @@
       <c r="E43">
         <v>236</v>
       </c>
-      <c r="F43" s="11">
-        <v>0.93055555555555547</v>
-      </c>
-      <c r="G43" s="2">
+      <c r="F43" s="11" t="n">
+        <v>0.9305555555555555</v>
+      </c>
+      <c r="G43" s="2" t="n">
         <v>44204</v>
       </c>
     </row>
@@ -4698,10 +4710,10 @@
       <c r="E44">
         <v>293</v>
       </c>
-      <c r="F44" s="11">
-        <v>0.97222222222222221</v>
-      </c>
-      <c r="G44" s="2">
+      <c r="F44" s="11" t="n">
+        <v>0.9722222222222222</v>
+      </c>
+      <c r="G44" s="2" t="n">
         <v>44205</v>
       </c>
     </row>
@@ -4721,10 +4733,10 @@
       <c r="E45">
         <v>101</v>
       </c>
-      <c r="F45" s="11">
-        <v>1.3888888888888888E-2</v>
-      </c>
-      <c r="G45" s="2">
+      <c r="F45" s="11" t="n">
+        <v>0.013888888888888888</v>
+      </c>
+      <c r="G45" s="2" t="n">
         <v>44206</v>
       </c>
     </row>
@@ -4744,10 +4756,10 @@
       <c r="E46">
         <v>223</v>
       </c>
-      <c r="F46" s="11">
-        <v>5.5555555555555552E-2</v>
-      </c>
-      <c r="G46" s="2">
+      <c r="F46" s="11" t="n">
+        <v>0.05555555555555555</v>
+      </c>
+      <c r="G46" s="2" t="n">
         <v>44207</v>
       </c>
     </row>
@@ -4767,10 +4779,10 @@
       <c r="E47">
         <v>202</v>
       </c>
-      <c r="F47" s="11">
-        <v>9.7222222222222224E-2</v>
-      </c>
-      <c r="G47" s="2">
+      <c r="F47" s="11" t="n">
+        <v>0.09722222222222222</v>
+      </c>
+      <c r="G47" s="2" t="n">
         <v>44208</v>
       </c>
     </row>
@@ -4790,10 +4802,10 @@
       <c r="E48">
         <v>361</v>
       </c>
-      <c r="F48" s="11">
+      <c r="F48" s="11" t="n">
         <v>0.1388888888888889</v>
       </c>
-      <c r="G48" s="2">
+      <c r="G48" s="2" t="n">
         <v>44209</v>
       </c>
     </row>
@@ -4813,10 +4825,10 @@
       <c r="E49">
         <v>103</v>
       </c>
-      <c r="F49" s="11">
+      <c r="F49" s="11" t="n">
         <v>0.18055555555555555</v>
       </c>
-      <c r="G49" s="2">
+      <c r="G49" s="2" t="n">
         <v>44210</v>
       </c>
     </row>
@@ -4836,10 +4848,10 @@
       <c r="E50">
         <v>379</v>
       </c>
-      <c r="F50" s="11">
-        <v>0.22222222222222221</v>
-      </c>
-      <c r="G50" s="2">
+      <c r="F50" s="11" t="n">
+        <v>0.2222222222222222</v>
+      </c>
+      <c r="G50" s="2" t="n">
         <v>44211</v>
       </c>
     </row>
@@ -4859,10 +4871,10 @@
       <c r="E51">
         <v>309</v>
       </c>
-      <c r="F51" s="11">
+      <c r="F51" s="11" t="n">
         <v>0.2638888888888889</v>
       </c>
-      <c r="G51" s="2">
+      <c r="G51" s="2" t="n">
         <v>44212</v>
       </c>
     </row>
@@ -4882,10 +4894,10 @@
       <c r="E52">
         <v>365</v>
       </c>
-      <c r="F52" s="11">
-        <v>0.30555555555555552</v>
-      </c>
-      <c r="G52" s="2">
+      <c r="F52" s="11" t="n">
+        <v>0.3055555555555555</v>
+      </c>
+      <c r="G52" s="2" t="n">
         <v>44213</v>
       </c>
     </row>
@@ -4905,10 +4917,10 @@
       <c r="E53">
         <v>259</v>
       </c>
-      <c r="F53" s="11">
+      <c r="F53" s="11" t="n">
         <v>0.34722222222222227</v>
       </c>
-      <c r="G53" s="2">
+      <c r="G53" s="2" t="n">
         <v>44214</v>
       </c>
     </row>
@@ -4928,10 +4940,10 @@
       <c r="E54">
         <v>227</v>
       </c>
-      <c r="F54" s="11">
+      <c r="F54" s="11" t="n">
         <v>0.3888888888888889</v>
       </c>
-      <c r="G54" s="2">
+      <c r="G54" s="2" t="n">
         <v>44215</v>
       </c>
     </row>
@@ -4951,10 +4963,10 @@
       <c r="E55">
         <v>105</v>
       </c>
-      <c r="F55" s="11">
-        <v>0.43055555555555558</v>
-      </c>
-      <c r="G55" s="2">
+      <c r="F55" s="11" t="n">
+        <v>0.4305555555555556</v>
+      </c>
+      <c r="G55" s="2" t="n">
         <v>44216</v>
       </c>
     </row>
@@ -4974,10 +4986,10 @@
       <c r="E56">
         <v>151</v>
       </c>
-      <c r="F56" s="11">
+      <c r="F56" s="11" t="n">
         <v>0.47222222222222227</v>
       </c>
-      <c r="G56" s="2">
+      <c r="G56" s="2" t="n">
         <v>44217</v>
       </c>
     </row>
@@ -4997,10 +5009,10 @@
       <c r="E57">
         <v>229</v>
       </c>
-      <c r="F57" s="11">
-        <v>0.51388888888888895</v>
-      </c>
-      <c r="G57" s="2">
+      <c r="F57" s="11" t="n">
+        <v>0.513888888888889</v>
+      </c>
+      <c r="G57" s="2" t="n">
         <v>44218</v>
       </c>
     </row>
@@ -5020,10 +5032,10 @@
       <c r="E58">
         <v>212</v>
       </c>
-      <c r="F58" s="11">
-        <v>0.55555555555555558</v>
-      </c>
-      <c r="G58" s="2">
+      <c r="F58" s="11" t="n">
+        <v>0.5555555555555556</v>
+      </c>
+      <c r="G58" s="2" t="n">
         <v>44219</v>
       </c>
     </row>
@@ -5043,10 +5055,10 @@
       <c r="E59">
         <v>310</v>
       </c>
-      <c r="F59" s="11">
-        <v>0.59722222222222221</v>
-      </c>
-      <c r="G59" s="2">
+      <c r="F59" s="11" t="n">
+        <v>0.5972222222222222</v>
+      </c>
+      <c r="G59" s="2" t="n">
         <v>44220</v>
       </c>
     </row>
@@ -5066,10 +5078,10 @@
       <c r="E60">
         <v>271</v>
       </c>
-      <c r="F60" s="11">
-        <v>0.63888888888888895</v>
-      </c>
-      <c r="G60" s="2">
+      <c r="F60" s="11" t="n">
+        <v>0.638888888888889</v>
+      </c>
+      <c r="G60" s="2" t="n">
         <v>44221</v>
       </c>
     </row>
@@ -5089,10 +5101,10 @@
       <c r="E61">
         <v>347</v>
       </c>
-      <c r="F61" s="11">
-        <v>0.68055555555555547</v>
-      </c>
-      <c r="G61" s="2">
+      <c r="F61" s="11" t="n">
+        <v>0.6805555555555555</v>
+      </c>
+      <c r="G61" s="2" t="n">
         <v>44222</v>
       </c>
     </row>
@@ -5112,10 +5124,10 @@
       <c r="E62">
         <v>351</v>
       </c>
-      <c r="F62" s="11">
-        <v>0.72222222222222221</v>
-      </c>
-      <c r="G62" s="2">
+      <c r="F62" s="11" t="n">
+        <v>0.7222222222222222</v>
+      </c>
+      <c r="G62" s="2" t="n">
         <v>44223</v>
       </c>
     </row>
@@ -5135,10 +5147,10 @@
       <c r="E63">
         <v>143</v>
       </c>
-      <c r="F63" s="11">
-        <v>0.76388888888888884</v>
-      </c>
-      <c r="G63" s="2">
+      <c r="F63" s="11" t="n">
+        <v>0.7638888888888888</v>
+      </c>
+      <c r="G63" s="2" t="n">
         <v>44224</v>
       </c>
     </row>
@@ -5158,10 +5170,10 @@
       <c r="E64">
         <v>140</v>
       </c>
-      <c r="F64" s="11">
-        <v>0.80555555555555547</v>
-      </c>
-      <c r="G64" s="2">
+      <c r="F64" s="11" t="n">
+        <v>0.8055555555555555</v>
+      </c>
+      <c r="G64" s="2" t="n">
         <v>44225</v>
       </c>
     </row>
@@ -5181,10 +5193,10 @@
       <c r="E65">
         <v>87</v>
       </c>
-      <c r="F65" s="11">
-        <v>0.84722222222222221</v>
-      </c>
-      <c r="G65" s="2">
+      <c r="F65" s="11" t="n">
+        <v>0.8472222222222222</v>
+      </c>
+      <c r="G65" s="2" t="n">
         <v>44226</v>
       </c>
     </row>
@@ -5204,10 +5216,10 @@
       <c r="E66">
         <v>132</v>
       </c>
-      <c r="F66" s="11">
-        <v>0.88888888888888884</v>
-      </c>
-      <c r="G66" s="2">
+      <c r="F66" s="11" t="n">
+        <v>0.8888888888888888</v>
+      </c>
+      <c r="G66" s="2" t="n">
         <v>44227</v>
       </c>
     </row>
@@ -5227,10 +5239,10 @@
       <c r="E67">
         <v>333</v>
       </c>
-      <c r="F67" s="11">
-        <v>0.93055555555555547</v>
-      </c>
-      <c r="G67" s="2">
+      <c r="F67" s="11" t="n">
+        <v>0.9305555555555555</v>
+      </c>
+      <c r="G67" s="2" t="n">
         <v>44228</v>
       </c>
     </row>
@@ -5250,10 +5262,10 @@
       <c r="E68">
         <v>141</v>
       </c>
-      <c r="F68" s="11">
-        <v>0.97222222222222221</v>
-      </c>
-      <c r="G68" s="2">
+      <c r="F68" s="11" t="n">
+        <v>0.9722222222222222</v>
+      </c>
+      <c r="G68" s="2" t="n">
         <v>44229</v>
       </c>
     </row>
@@ -5273,10 +5285,10 @@
       <c r="E69">
         <v>99</v>
       </c>
-      <c r="F69" s="11">
-        <v>1.3888888888888888E-2</v>
-      </c>
-      <c r="G69" s="2">
+      <c r="F69" s="11" t="n">
+        <v>0.013888888888888888</v>
+      </c>
+      <c r="G69" s="2" t="n">
         <v>44230</v>
       </c>
     </row>
@@ -5296,10 +5308,10 @@
       <c r="E70">
         <v>195</v>
       </c>
-      <c r="F70" s="11">
-        <v>5.5555555555555552E-2</v>
-      </c>
-      <c r="G70" s="2">
+      <c r="F70" s="11" t="n">
+        <v>0.05555555555555555</v>
+      </c>
+      <c r="G70" s="2" t="n">
         <v>44231</v>
       </c>
     </row>
@@ -5319,10 +5331,10 @@
       <c r="E71">
         <v>261</v>
       </c>
-      <c r="F71" s="11">
-        <v>9.7222222222222224E-2</v>
-      </c>
-      <c r="G71" s="2">
+      <c r="F71" s="11" t="n">
+        <v>0.09722222222222222</v>
+      </c>
+      <c r="G71" s="2" t="n">
         <v>44232</v>
       </c>
     </row>
@@ -5342,10 +5354,10 @@
       <c r="E72">
         <v>277</v>
       </c>
-      <c r="F72" s="11">
+      <c r="F72" s="11" t="n">
         <v>0.1388888888888889</v>
       </c>
-      <c r="G72" s="2">
+      <c r="G72" s="2" t="n">
         <v>44233</v>
       </c>
     </row>
@@ -5365,10 +5377,10 @@
       <c r="E73">
         <v>190</v>
       </c>
-      <c r="F73" s="11">
+      <c r="F73" s="11" t="n">
         <v>0.18055555555555555</v>
       </c>
-      <c r="G73" s="2">
+      <c r="G73" s="2" t="n">
         <v>44234</v>
       </c>
     </row>
@@ -5388,10 +5400,10 @@
       <c r="E74">
         <v>88</v>
       </c>
-      <c r="F74" s="11">
-        <v>0.22222222222222221</v>
-      </c>
-      <c r="G74" s="2">
+      <c r="F74" s="11" t="n">
+        <v>0.2222222222222222</v>
+      </c>
+      <c r="G74" s="2" t="n">
         <v>44235</v>
       </c>
     </row>
@@ -5411,10 +5423,10 @@
       <c r="E75">
         <v>278</v>
       </c>
-      <c r="F75" s="11">
+      <c r="F75" s="11" t="n">
         <v>0.2638888888888889</v>
       </c>
-      <c r="G75" s="2">
+      <c r="G75" s="2" t="n">
         <v>44236</v>
       </c>
     </row>
@@ -5434,10 +5446,10 @@
       <c r="E76">
         <v>305</v>
       </c>
-      <c r="F76" s="11">
-        <v>0.30555555555555552</v>
-      </c>
-      <c r="G76" s="2">
+      <c r="F76" s="11" t="n">
+        <v>0.3055555555555555</v>
+      </c>
+      <c r="G76" s="2" t="n">
         <v>44237</v>
       </c>
     </row>
@@ -5457,10 +5469,10 @@
       <c r="E77">
         <v>128</v>
       </c>
-      <c r="F77" s="11">
+      <c r="F77" s="11" t="n">
         <v>0.34722222222222227</v>
       </c>
-      <c r="G77" s="2">
+      <c r="G77" s="2" t="n">
         <v>44238</v>
       </c>
     </row>
@@ -5480,10 +5492,10 @@
       <c r="E78">
         <v>82</v>
       </c>
-      <c r="F78" s="11">
+      <c r="F78" s="11" t="n">
         <v>0.3888888888888889</v>
       </c>
-      <c r="G78" s="2">
+      <c r="G78" s="2" t="n">
         <v>44239</v>
       </c>
     </row>
@@ -5503,16 +5515,58 @@
       <c r="E79">
         <v>403</v>
       </c>
-      <c r="F79" s="15">
-        <v>7.1527777777777801E-2</v>
-      </c>
-      <c r="G79" s="17">
+      <c r="F79" s="15" t="n">
+        <v>0.0715277777777778</v>
+      </c>
+      <c r="G79" s="16" t="n">
         <v>44312</v>
       </c>
     </row>
     <row r="80" spans="1:7">
-      <c r="F80" s="15"/>
-      <c r="G80" s="16"/>
+      <c r="A80">
+        <v>80</v>
+      </c>
+      <c r="B80" t="s">
+        <v>237</v>
+      </c>
+      <c r="C80" t="s">
+        <v>259</v>
+      </c>
+      <c r="D80">
+        <v>3</v>
+      </c>
+      <c r="E80">
+        <v>457</v>
+      </c>
+      <c r="F80" s="15" t="n">
+        <v>0.109027777777778</v>
+      </c>
+      <c r="G80" s="16" t="n">
+        <v>44312</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7">
+      <c r="A81" t="n">
+        <v>82</v>
+      </c>
+      <c r="B81" t="s">
+        <v>237</v>
+      </c>
+      <c r="C81" t="s">
+        <v>298</v>
+      </c>
+      <c r="D81" t="n">
+        <v>3</v>
+      </c>
+      <c r="E81" t="n">
+        <v>459</v>
+      </c>
+      <c r="F81" s="15" t="n">
+        <v>0.110416666666667</v>
+      </c>
+      <c r="G81" s="18" t="n">
+        <v>44312</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5525,7 +5579,7 @@
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="4" t="s">
@@ -5554,7 +5608,7 @@
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="4" t="s">
@@ -5583,7 +5637,7 @@
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="4" t="s">
@@ -5612,7 +5666,7 @@
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="4" t="s">
@@ -5641,7 +5695,7 @@
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="4" t="s">
@@ -5670,7 +5724,7 @@
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="4" t="s">
@@ -5699,7 +5753,7 @@
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="4" t="s">
@@ -5728,7 +5782,7 @@
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="4" t="s">
@@ -5757,7 +5811,7 @@
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="4" t="s">
@@ -5791,7 +5845,7 @@
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="4" t="s">
@@ -5811,13 +5865,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="9.6640625" customWidth="1"/>
     <col min="3" max="3" width="9.44140625" customWidth="1"/>
@@ -5826,7 +5878,7 @@
     <col min="9" max="9" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1">
       <c r="A1" s="4" t="s">
         <v>109</v>
       </c>
@@ -5858,28 +5910,153 @@
         <v>258</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
-      <c r="F2" s="15"/>
-      <c r="G2" s="16"/>
-      <c r="J2">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="F3" s="15"/>
-      <c r="G3" s="16"/>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="F4" s="15"/>
-      <c r="G4" s="16"/>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="F5" s="15"/>
-      <c r="G5" s="16"/>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="F6" s="15"/>
-      <c r="G6" s="16"/>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>300</v>
+      </c>
+      <c r="B2" t="s">
+        <v>300</v>
+      </c>
+      <c r="C2" t="s">
+        <v>300</v>
+      </c>
+      <c r="D2" t="s">
+        <v>300</v>
+      </c>
+      <c r="E2" t="s">
+        <v>300</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>300</v>
+      </c>
+      <c r="G2" s="16" t="s">
+        <v>300</v>
+      </c>
+      <c r="H2" t="s">
+        <v>300</v>
+      </c>
+      <c r="I2" t="s">
+        <v>300</v>
+      </c>
+      <c r="J2" t="n">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+    </row>
+    <row r="4">
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+    </row>
+    <row r="5">
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
+    </row>
+    <row r="6">
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
+    </row>
+    <row r="7">
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
+    </row>
+    <row r="8">
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
+    </row>
+    <row r="9">
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
+    </row>
+    <row r="10">
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
+    </row>
+    <row r="11">
+      <c r="F11" s="17"/>
+      <c r="G11" s="17"/>
+    </row>
+    <row r="12">
+      <c r="F12" s="17"/>
+      <c r="G12" s="17"/>
+    </row>
+    <row r="13">
+      <c r="F13" s="17"/>
+      <c r="G13" s="17"/>
+    </row>
+    <row r="14">
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+    </row>
+    <row r="15">
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
+    </row>
+    <row r="16">
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
+    </row>
+    <row r="17" spans="6:7">
+      <c r="F17" s="17"/>
+      <c r="G17" s="17"/>
+    </row>
+    <row r="18" spans="6:7">
+      <c r="F18" s="17"/>
+      <c r="G18" s="17"/>
+    </row>
+    <row r="19" spans="6:7">
+      <c r="F19" s="17"/>
+      <c r="G19" s="17"/>
+    </row>
+    <row r="20" spans="6:7">
+      <c r="F20" s="17"/>
+      <c r="G20" s="17"/>
+    </row>
+    <row r="21" spans="6:7">
+      <c r="F21" s="17"/>
+      <c r="G21" s="17"/>
+    </row>
+    <row r="22" spans="6:7">
+      <c r="F22" s="17"/>
+      <c r="G22" s="17"/>
+    </row>
+    <row r="23" spans="6:7">
+      <c r="F23" s="17"/>
+      <c r="G23" s="17"/>
+    </row>
+    <row r="24" spans="6:7">
+      <c r="F24" s="17"/>
+      <c r="G24" s="17"/>
+    </row>
+    <row r="25" spans="6:7">
+      <c r="F25" s="17"/>
+      <c r="G25" s="17"/>
+    </row>
+    <row r="26" spans="6:7">
+      <c r="F26" s="17"/>
+      <c r="G26" s="17"/>
+    </row>
+    <row r="27" spans="6:7">
+      <c r="F27" s="17"/>
+      <c r="G27" s="17"/>
+    </row>
+    <row r="28" spans="6:7">
+      <c r="F28" s="17"/>
+      <c r="G28" s="17"/>
+    </row>
+    <row r="29" spans="6:7">
+      <c r="F29" s="17"/>
+      <c r="G29" s="17"/>
+    </row>
+    <row r="30" spans="6:7">
+      <c r="F30" s="17"/>
+      <c r="G30" s="17"/>
+    </row>
+    <row r="31" spans="6:7">
+      <c r="F31" s="17"/>
+      <c r="G31" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5892,7 +6069,7 @@
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="4" t="s">
@@ -5916,7 +6093,7 @@
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="4" t="s">
@@ -5940,7 +6117,7 @@
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="4" t="s">
@@ -5964,7 +6141,7 @@
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="4" t="s">
@@ -5988,7 +6165,7 @@
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="4" t="s">
@@ -6012,7 +6189,7 @@
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="4" t="s">
@@ -6036,7 +6213,7 @@
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="4" t="s">
@@ -6060,7 +6237,7 @@
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="4" t="s">
@@ -6084,7 +6261,7 @@
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="4" t="s">
@@ -6108,7 +6285,7 @@
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="4" t="s">
@@ -6166,11 +6343,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="8" max="8" width="6" customWidth="1"/>
   </cols>
@@ -6214,6 +6391,22 @@
       </c>
       <c r="C4" t="s">
         <v>261</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>80</v>
+      </c>
+      <c r="B5" t="s">
+        <v>298</v>
+      </c>
+      <c r="C5" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="n">
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -6227,7 +6420,7 @@
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="4" t="s">
@@ -6289,7 +6482,7 @@
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="4" t="s">
@@ -6342,11 +6535,11 @@
 
 <file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="4" t="s">
@@ -6400,6 +6593,16 @@
     <row r="6" spans="1:5">
       <c r="A6">
         <v>78</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="n">
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -6413,7 +6616,7 @@
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="4" t="s">
@@ -6470,7 +6673,7 @@
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="4" t="s">
@@ -6527,7 +6730,7 @@
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="4" t="s">
@@ -6567,7 +6770,7 @@
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="4" t="s">
@@ -6611,7 +6814,7 @@
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="4" t="s">
@@ -6640,7 +6843,7 @@
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="4" t="s">

</xml_diff>

<commit_message>
ADD: admin class and dataBase
</commit_message>
<xml_diff>
--- a/build-PSS_HomeWork4-Desktop_Qt_5_12_5_MinGW_64_bit-Release/release/DataBase/Accounts.xlsx
+++ b/build-PSS_HomeWork4-Desktop_Qt_5_12_5_MinGW_64_bit-Release/release/DataBase/Accounts.xlsx
@@ -4,70 +4,71 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="51"/>
+    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Passenger" sheetId="1" r:id="rId1"/>
     <sheet name="Driver" sheetId="2" r:id="rId2"/>
-    <sheet name="Orders" sheetId="47" r:id="rId3"/>
-    <sheet name="Active_orders" sheetId="54" r:id="rId4"/>
-    <sheet name="89959280771" sheetId="3" r:id="rId5"/>
-    <sheet name="89180884879" sheetId="4" r:id="rId6"/>
-    <sheet name="89962840843" sheetId="5" r:id="rId7"/>
-    <sheet name="89313306966" sheetId="6" r:id="rId8"/>
-    <sheet name="89306140496" sheetId="7" r:id="rId9"/>
-    <sheet name="89394702333" sheetId="8" r:id="rId10"/>
-    <sheet name="89833750451" sheetId="9" r:id="rId11"/>
-    <sheet name="89787150096" sheetId="10" r:id="rId12"/>
-    <sheet name="89992098153" sheetId="11" r:id="rId13"/>
-    <sheet name="89268200405" sheetId="12" r:id="rId14"/>
-    <sheet name="89926260702" sheetId="13" r:id="rId15"/>
-    <sheet name="89492911777" sheetId="14" r:id="rId16"/>
-    <sheet name="89330959189" sheetId="15" r:id="rId17"/>
-    <sheet name="89423670770" sheetId="16" r:id="rId18"/>
-    <sheet name="89185241280" sheetId="17" r:id="rId19"/>
-    <sheet name="89990916326" sheetId="18" r:id="rId20"/>
-    <sheet name="89673329996" sheetId="19" r:id="rId21"/>
-    <sheet name="89202864668" sheetId="20" r:id="rId22"/>
-    <sheet name="89601579888" sheetId="21" r:id="rId23"/>
-    <sheet name="89607860943" sheetId="22" r:id="rId24"/>
-    <sheet name="89231886764" sheetId="23" r:id="rId25"/>
-    <sheet name="89539860223" sheetId="24" r:id="rId26"/>
-    <sheet name="89959405648" sheetId="25" r:id="rId27"/>
-    <sheet name="89705356787" sheetId="26" r:id="rId28"/>
-    <sheet name="89832868047" sheetId="27" r:id="rId29"/>
-    <sheet name="89282911827" sheetId="28" r:id="rId30"/>
-    <sheet name="89214352791" sheetId="29" r:id="rId31"/>
-    <sheet name="89133279195" sheetId="30" r:id="rId32"/>
-    <sheet name="89292850692" sheetId="31" r:id="rId33"/>
-    <sheet name="89695933467" sheetId="32" r:id="rId34"/>
-    <sheet name="89278666277" sheetId="33" r:id="rId35"/>
-    <sheet name="89871022956" sheetId="34" r:id="rId36"/>
-    <sheet name="89797832254" sheetId="35" r:id="rId37"/>
-    <sheet name="89281242037" sheetId="36" r:id="rId38"/>
-    <sheet name="89177853860" sheetId="37" r:id="rId39"/>
-    <sheet name="89793704898" sheetId="38" r:id="rId40"/>
-    <sheet name="89624920064" sheetId="39" r:id="rId41"/>
-    <sheet name="89532136828" sheetId="40" r:id="rId42"/>
-    <sheet name="89869988648" sheetId="41" r:id="rId43"/>
-    <sheet name="89767989697" sheetId="42" r:id="rId44"/>
-    <sheet name="89985042567" sheetId="43" r:id="rId45"/>
-    <sheet name="89488486412" sheetId="44" r:id="rId46"/>
-    <sheet name="89297310394" sheetId="45" r:id="rId47"/>
-    <sheet name="89286091054" sheetId="46" r:id="rId48"/>
-    <sheet name="333223827" sheetId="48" r:id="rId49"/>
-    <sheet name="333223322" sheetId="49" r:id="rId50"/>
-    <sheet name="333225555" sheetId="50" r:id="rId51"/>
-    <sheet name="333221234" sheetId="51" r:id="rId52"/>
-    <sheet name="333227531" sheetId="52" r:id="rId53"/>
-    <sheet name="333220011" sheetId="53" r:id="rId54"/>
+    <sheet name="Admin" sheetId="55" r:id="rId3"/>
+    <sheet name="Orders" sheetId="47" r:id="rId4"/>
+    <sheet name="Active_orders" sheetId="54" r:id="rId5"/>
+    <sheet name="89959280771" sheetId="3" r:id="rId6"/>
+    <sheet name="89180884879" sheetId="4" r:id="rId7"/>
+    <sheet name="89962840843" sheetId="5" r:id="rId8"/>
+    <sheet name="89313306966" sheetId="6" r:id="rId9"/>
+    <sheet name="89306140496" sheetId="7" r:id="rId10"/>
+    <sheet name="89394702333" sheetId="8" r:id="rId11"/>
+    <sheet name="89833750451" sheetId="9" r:id="rId12"/>
+    <sheet name="89787150096" sheetId="10" r:id="rId13"/>
+    <sheet name="89992098153" sheetId="11" r:id="rId14"/>
+    <sheet name="89268200405" sheetId="12" r:id="rId15"/>
+    <sheet name="89926260702" sheetId="13" r:id="rId16"/>
+    <sheet name="89492911777" sheetId="14" r:id="rId17"/>
+    <sheet name="89330959189" sheetId="15" r:id="rId18"/>
+    <sheet name="89423670770" sheetId="16" r:id="rId19"/>
+    <sheet name="89185241280" sheetId="17" r:id="rId20"/>
+    <sheet name="89990916326" sheetId="18" r:id="rId21"/>
+    <sheet name="89673329996" sheetId="19" r:id="rId22"/>
+    <sheet name="89202864668" sheetId="20" r:id="rId23"/>
+    <sheet name="89601579888" sheetId="21" r:id="rId24"/>
+    <sheet name="89607860943" sheetId="22" r:id="rId25"/>
+    <sheet name="89231886764" sheetId="23" r:id="rId26"/>
+    <sheet name="89539860223" sheetId="24" r:id="rId27"/>
+    <sheet name="89959405648" sheetId="25" r:id="rId28"/>
+    <sheet name="89705356787" sheetId="26" r:id="rId29"/>
+    <sheet name="89832868047" sheetId="27" r:id="rId30"/>
+    <sheet name="89282911827" sheetId="28" r:id="rId31"/>
+    <sheet name="89214352791" sheetId="29" r:id="rId32"/>
+    <sheet name="89133279195" sheetId="30" r:id="rId33"/>
+    <sheet name="89292850692" sheetId="31" r:id="rId34"/>
+    <sheet name="89695933467" sheetId="32" r:id="rId35"/>
+    <sheet name="89278666277" sheetId="33" r:id="rId36"/>
+    <sheet name="89871022956" sheetId="34" r:id="rId37"/>
+    <sheet name="89797832254" sheetId="35" r:id="rId38"/>
+    <sheet name="89281242037" sheetId="36" r:id="rId39"/>
+    <sheet name="89177853860" sheetId="37" r:id="rId40"/>
+    <sheet name="89793704898" sheetId="38" r:id="rId41"/>
+    <sheet name="89624920064" sheetId="39" r:id="rId42"/>
+    <sheet name="89532136828" sheetId="40" r:id="rId43"/>
+    <sheet name="89869988648" sheetId="41" r:id="rId44"/>
+    <sheet name="89767989697" sheetId="42" r:id="rId45"/>
+    <sheet name="89985042567" sheetId="43" r:id="rId46"/>
+    <sheet name="89488486412" sheetId="44" r:id="rId47"/>
+    <sheet name="89297310394" sheetId="45" r:id="rId48"/>
+    <sheet name="89286091054" sheetId="46" r:id="rId49"/>
+    <sheet name="333223827" sheetId="48" r:id="rId50"/>
+    <sheet name="333223322" sheetId="49" r:id="rId51"/>
+    <sheet name="333225555" sheetId="50" r:id="rId52"/>
+    <sheet name="333221234" sheetId="51" r:id="rId53"/>
+    <sheet name="333227531" sheetId="52" r:id="rId54"/>
+    <sheet name="333220011" sheetId="53" r:id="rId55"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="302">
   <si>
     <t>Leroy</t>
   </si>
@@ -983,51 +984,53 @@
     <t>st. Raisoveta, 8</t>
   </si>
   <si>
-    <t>89959280771</t>
-  </si>
-  <si>
     <t/>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Boss </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="hh:mm:ss"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
-    <numFmt numFmtId="176" formatCode="yyyy-mm-dd"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <charset val="204"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF800080"/>
       <name val="Arial Unicode MS"/>
+      <family val="2"/>
       <charset val="204"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FFC0C0C0"/>
       <name val="Arial Unicode MS"/>
+      <family val="2"/>
       <charset val="204"/>
-      <family val="2"/>
     </font>
     <font>
       <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <charset val="204"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1041,9 +1044,6 @@
       <color rgb="FFC0C0C0"/>
       <name val="Arial Unicode MS"/>
       <family val="2"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="5">
@@ -1173,7 +1173,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1200,10 +1200,11 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1497,9 +1498,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="8.109375" customWidth="1"/>
     <col min="2" max="2" width="9.5546875" customWidth="1"/>
@@ -1512,7 +1515,7 @@
     <col min="9" max="9" width="10.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:8">
       <c r="A1" s="3" t="s">
         <v>87</v>
       </c>
@@ -1538,7 +1541,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>262</v>
       </c>
@@ -1548,7 +1551,7 @@
       <c r="C2" t="s">
         <v>90</v>
       </c>
-      <c r="D2" s="2" t="n">
+      <c r="D2" s="2">
         <v>23864</v>
       </c>
       <c r="E2">
@@ -1564,7 +1567,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -1574,7 +1577,7 @@
       <c r="C3" t="s">
         <v>90</v>
       </c>
-      <c r="D3" s="2" t="n">
+      <c r="D3" s="2">
         <v>26467</v>
       </c>
       <c r="E3">
@@ -1590,7 +1593,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -1600,7 +1603,7 @@
       <c r="C4" t="s">
         <v>90</v>
       </c>
-      <c r="D4" s="2" t="n">
+      <c r="D4" s="2">
         <v>31167</v>
       </c>
       <c r="E4">
@@ -1616,7 +1619,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -1626,7 +1629,7 @@
       <c r="C5" t="s">
         <v>90</v>
       </c>
-      <c r="D5" s="2" t="n">
+      <c r="D5" s="2">
         <v>32852</v>
       </c>
       <c r="E5">
@@ -1642,7 +1645,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -1652,7 +1655,7 @@
       <c r="C6" t="s">
         <v>90</v>
       </c>
-      <c r="D6" s="2" t="n">
+      <c r="D6" s="2">
         <v>26494</v>
       </c>
       <c r="E6">
@@ -1668,7 +1671,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -1678,7 +1681,7 @@
       <c r="C7" t="s">
         <v>91</v>
       </c>
-      <c r="D7" s="2" t="n">
+      <c r="D7" s="2">
         <v>33284</v>
       </c>
       <c r="E7">
@@ -1694,7 +1697,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -1704,7 +1707,7 @@
       <c r="C8" t="s">
         <v>91</v>
       </c>
-      <c r="D8" s="2" t="n">
+      <c r="D8" s="2">
         <v>27334</v>
       </c>
       <c r="E8">
@@ -1720,7 +1723,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -1730,7 +1733,7 @@
       <c r="C9" t="s">
         <v>90</v>
       </c>
-      <c r="D9" s="2" t="n">
+      <c r="D9" s="2">
         <v>37211</v>
       </c>
       <c r="E9">
@@ -1746,7 +1749,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -1756,7 +1759,7 @@
       <c r="C10" t="s">
         <v>90</v>
       </c>
-      <c r="D10" s="2" t="n">
+      <c r="D10" s="2">
         <v>28951</v>
       </c>
       <c r="E10">
@@ -1772,7 +1775,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:8">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -1782,7 +1785,7 @@
       <c r="C11" t="s">
         <v>90</v>
       </c>
-      <c r="D11" s="2" t="n">
+      <c r="D11" s="2">
         <v>30962</v>
       </c>
       <c r="E11">
@@ -1798,7 +1801,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:8">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -1808,7 +1811,7 @@
       <c r="C12" t="s">
         <v>91</v>
       </c>
-      <c r="D12" s="2" t="n">
+      <c r="D12" s="2">
         <v>37478</v>
       </c>
       <c r="E12">
@@ -1824,7 +1827,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:8">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -1834,7 +1837,7 @@
       <c r="C13" t="s">
         <v>91</v>
       </c>
-      <c r="D13" s="2" t="n">
+      <c r="D13" s="2">
         <v>35118</v>
       </c>
       <c r="E13">
@@ -1850,7 +1853,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:8">
       <c r="A14" t="s">
         <v>1</v>
       </c>
@@ -1860,7 +1863,7 @@
       <c r="C14" t="s">
         <v>90</v>
       </c>
-      <c r="D14" s="2" t="n">
+      <c r="D14" s="2">
         <v>24495</v>
       </c>
       <c r="E14">
@@ -1876,7 +1879,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:8">
       <c r="A15" t="s">
         <v>10</v>
       </c>
@@ -1886,7 +1889,7 @@
       <c r="C15" t="s">
         <v>90</v>
       </c>
-      <c r="D15" s="2" t="n">
+      <c r="D15" s="2">
         <v>27707</v>
       </c>
       <c r="E15">
@@ -1902,7 +1905,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:8">
       <c r="A16" t="s">
         <v>11</v>
       </c>
@@ -1912,7 +1915,7 @@
       <c r="C16" t="s">
         <v>90</v>
       </c>
-      <c r="D16" s="2" t="n">
+      <c r="D16" s="2">
         <v>34909</v>
       </c>
       <c r="E16">
@@ -1938,7 +1941,7 @@
       <c r="C17" t="s">
         <v>90</v>
       </c>
-      <c r="D17" s="2" t="n">
+      <c r="D17" s="2">
         <v>27606</v>
       </c>
       <c r="E17">
@@ -1964,7 +1967,7 @@
       <c r="C18" t="s">
         <v>90</v>
       </c>
-      <c r="D18" s="2" t="n">
+      <c r="D18" s="2">
         <v>26204</v>
       </c>
       <c r="E18">
@@ -1990,7 +1993,7 @@
       <c r="C19" t="s">
         <v>90</v>
       </c>
-      <c r="D19" s="2" t="n">
+      <c r="D19" s="2">
         <v>24456</v>
       </c>
       <c r="E19">
@@ -2016,7 +2019,7 @@
       <c r="C20" t="s">
         <v>91</v>
       </c>
-      <c r="D20" s="2" t="n">
+      <c r="D20" s="2">
         <v>25617</v>
       </c>
       <c r="E20">
@@ -2042,7 +2045,7 @@
       <c r="C21" t="s">
         <v>90</v>
       </c>
-      <c r="D21" s="2" t="n">
+      <c r="D21" s="2">
         <v>30392</v>
       </c>
       <c r="E21">
@@ -2068,7 +2071,7 @@
       <c r="C22" t="s">
         <v>91</v>
       </c>
-      <c r="D22" s="2" t="n">
+      <c r="D22" s="2">
         <v>34683</v>
       </c>
       <c r="E22">
@@ -2094,7 +2097,7 @@
       <c r="C23" t="s">
         <v>91</v>
       </c>
-      <c r="D23" s="2" t="n">
+      <c r="D23" s="2">
         <v>29643</v>
       </c>
       <c r="E23">
@@ -2120,7 +2123,7 @@
       <c r="C24" t="s">
         <v>91</v>
       </c>
-      <c r="D24" s="2" t="n">
+      <c r="D24" s="2">
         <v>33276</v>
       </c>
       <c r="E24">
@@ -2146,7 +2149,7 @@
       <c r="C25" t="s">
         <v>90</v>
       </c>
-      <c r="D25" s="2" t="n">
+      <c r="D25" s="2">
         <v>27002</v>
       </c>
       <c r="E25">
@@ -2172,7 +2175,7 @@
       <c r="C26" t="s">
         <v>91</v>
       </c>
-      <c r="D26" s="2" t="n">
+      <c r="D26" s="2">
         <v>36440</v>
       </c>
       <c r="E26">
@@ -2198,7 +2201,7 @@
       <c r="C27" t="s">
         <v>90</v>
       </c>
-      <c r="D27" s="2" t="n">
+      <c r="D27" s="2">
         <v>26848</v>
       </c>
       <c r="E27">
@@ -2224,7 +2227,7 @@
       <c r="C28" t="s">
         <v>91</v>
       </c>
-      <c r="D28" s="2" t="n">
+      <c r="D28" s="2">
         <v>36235</v>
       </c>
       <c r="E28">
@@ -2250,7 +2253,7 @@
       <c r="C29" t="s">
         <v>90</v>
       </c>
-      <c r="D29" s="2" t="n">
+      <c r="D29" s="2">
         <v>27142</v>
       </c>
       <c r="E29">
@@ -2276,7 +2279,7 @@
       <c r="C30" t="s">
         <v>91</v>
       </c>
-      <c r="D30" s="2" t="n">
+      <c r="D30" s="2">
         <v>22558</v>
       </c>
       <c r="E30">
@@ -2302,7 +2305,7 @@
       <c r="C31" t="s">
         <v>90</v>
       </c>
-      <c r="D31" s="2" t="n">
+      <c r="D31" s="2">
         <v>31838</v>
       </c>
       <c r="E31">
@@ -2328,7 +2331,7 @@
       <c r="C32" t="s">
         <v>90</v>
       </c>
-      <c r="D32" s="2" t="n">
+      <c r="D32" s="2">
         <v>35991</v>
       </c>
       <c r="E32">
@@ -2354,7 +2357,7 @@
       <c r="C33" t="s">
         <v>90</v>
       </c>
-      <c r="D33" s="2" t="n">
+      <c r="D33" s="2">
         <v>29065</v>
       </c>
       <c r="E33">
@@ -2380,7 +2383,7 @@
       <c r="C34" t="s">
         <v>90</v>
       </c>
-      <c r="D34" s="2" t="n">
+      <c r="D34" s="2">
         <v>31282</v>
       </c>
       <c r="E34">
@@ -2406,7 +2409,7 @@
       <c r="C35" t="s">
         <v>91</v>
       </c>
-      <c r="D35" s="2" t="n">
+      <c r="D35" s="2">
         <v>22663</v>
       </c>
       <c r="E35">
@@ -2432,7 +2435,7 @@
       <c r="C36" t="s">
         <v>91</v>
       </c>
-      <c r="D36" s="2" t="n">
+      <c r="D36" s="2">
         <v>33782</v>
       </c>
       <c r="E36">
@@ -2458,7 +2461,7 @@
       <c r="C37" t="s">
         <v>90</v>
       </c>
-      <c r="D37" s="2" t="n">
+      <c r="D37" s="2">
         <v>34169</v>
       </c>
       <c r="E37">
@@ -2484,7 +2487,7 @@
       <c r="C38" t="s">
         <v>90</v>
       </c>
-      <c r="D38" s="2" t="n">
+      <c r="D38" s="2">
         <v>25868</v>
       </c>
       <c r="E38">
@@ -2510,7 +2513,7 @@
       <c r="C39" t="s">
         <v>90</v>
       </c>
-      <c r="D39" s="2" t="n">
+      <c r="D39" s="2">
         <v>27197</v>
       </c>
       <c r="E39">
@@ -2536,7 +2539,7 @@
       <c r="C40" t="s">
         <v>91</v>
       </c>
-      <c r="D40" s="2" t="n">
+      <c r="D40" s="2">
         <v>31031</v>
       </c>
       <c r="E40">
@@ -2562,7 +2565,7 @@
       <c r="C41" t="s">
         <v>91</v>
       </c>
-      <c r="D41" s="2" t="n">
+      <c r="D41" s="2">
         <v>24333</v>
       </c>
       <c r="E41">
@@ -2588,7 +2591,7 @@
       <c r="C42" t="s">
         <v>91</v>
       </c>
-      <c r="D42" s="2" t="n">
+      <c r="D42" s="2">
         <v>30275</v>
       </c>
       <c r="E42">
@@ -2614,7 +2617,7 @@
       <c r="C43" t="s">
         <v>90</v>
       </c>
-      <c r="D43" s="2" t="n">
+      <c r="D43" s="2">
         <v>29192</v>
       </c>
       <c r="E43">
@@ -2640,7 +2643,7 @@
       <c r="C44" t="s">
         <v>90</v>
       </c>
-      <c r="D44" s="2" t="n">
+      <c r="D44" s="2">
         <v>29973</v>
       </c>
       <c r="E44">
@@ -2666,7 +2669,7 @@
       <c r="C45" t="s">
         <v>90</v>
       </c>
-      <c r="D45" s="2" t="n">
+      <c r="D45" s="2">
         <v>31402</v>
       </c>
       <c r="E45">
@@ -2693,7 +2696,7 @@
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="4" t="s">
@@ -2708,7 +2711,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -2718,11 +2721,11 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="4" t="s">
@@ -2737,17 +2740,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -2761,7 +2754,7 @@
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="4" t="s">
@@ -2776,17 +2769,17 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -2800,7 +2793,7 @@
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="4" t="s">
@@ -2815,17 +2808,17 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -2839,7 +2832,7 @@
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="4" t="s">
@@ -2854,17 +2847,17 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -2878,7 +2871,7 @@
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="4" t="s">
@@ -2893,17 +2886,17 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -2917,7 +2910,7 @@
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="4" t="s">
@@ -2932,17 +2925,17 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -2956,7 +2949,7 @@
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="4" t="s">
@@ -2971,17 +2964,17 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -2995,7 +2988,7 @@
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="4" t="s">
@@ -3010,17 +3003,17 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -3034,7 +3027,7 @@
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="4" t="s">
@@ -3049,17 +3042,17 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -3073,7 +3066,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="3" max="3" width="6.6640625" customWidth="1"/>
     <col min="4" max="4" width="11.33203125" customWidth="1"/>
@@ -3118,7 +3111,7 @@
       <c r="C2" t="s">
         <v>91</v>
       </c>
-      <c r="D2" s="2" t="n">
+      <c r="D2" s="2">
         <v>35888</v>
       </c>
       <c r="E2">
@@ -3144,7 +3137,7 @@
       <c r="C3" t="s">
         <v>91</v>
       </c>
-      <c r="D3" s="2" t="n">
+      <c r="D3" s="2">
         <v>26607</v>
       </c>
       <c r="E3">
@@ -3170,7 +3163,7 @@
       <c r="C4" t="s">
         <v>91</v>
       </c>
-      <c r="D4" s="2" t="n">
+      <c r="D4" s="2">
         <v>36103</v>
       </c>
       <c r="E4">
@@ -3196,7 +3189,7 @@
       <c r="C5" t="s">
         <v>90</v>
       </c>
-      <c r="D5" s="2" t="n">
+      <c r="D5" s="2">
         <v>32991</v>
       </c>
       <c r="E5">
@@ -3222,7 +3215,7 @@
       <c r="C6" t="s">
         <v>90</v>
       </c>
-      <c r="D6" s="2" t="n">
+      <c r="D6" s="2">
         <v>35858</v>
       </c>
       <c r="E6">
@@ -3248,7 +3241,7 @@
       <c r="C7" t="s">
         <v>90</v>
       </c>
-      <c r="D7" s="2" t="n">
+      <c r="D7" s="2">
         <v>24559</v>
       </c>
       <c r="E7">
@@ -3275,7 +3268,7 @@
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="4" t="s">
@@ -3290,17 +3283,17 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -3314,7 +3307,7 @@
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="4" t="s">
@@ -3329,17 +3322,17 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -3353,7 +3346,7 @@
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="4" t="s">
@@ -3368,17 +3361,17 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -3388,11 +3381,11 @@
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="4" t="s">
@@ -3407,22 +3400,17 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -3436,7 +3424,7 @@
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="4" t="s">
@@ -3451,22 +3439,22 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -3476,11 +3464,11 @@
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="4" t="s">
@@ -3495,17 +3483,22 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4">
-        <v>58</v>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -3515,11 +3508,11 @@
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="4" t="s">
@@ -3534,12 +3527,17 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3">
-        <v>60</v>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -3549,11 +3547,11 @@
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="4" t="s">
@@ -3568,17 +3566,12 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -3588,11 +3581,11 @@
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="4" t="s">
@@ -3607,12 +3600,17 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3">
-        <v>65</v>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -3626,7 +3624,7 @@
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="4" t="s">
@@ -3641,12 +3639,12 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -3656,11 +3654,409 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="H1" s="19"/>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
+        <v>300</v>
+      </c>
+      <c r="B2" t="s">
+        <v>301</v>
+      </c>
+      <c r="C2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D2" s="2">
+        <v>31257</v>
+      </c>
+      <c r="E2" s="19">
+        <v>4223</v>
+      </c>
+      <c r="F2">
+        <v>191439</v>
+      </c>
+      <c r="G2">
+        <v>3377722</v>
+      </c>
+      <c r="H2" s="19"/>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="19"/>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="H6" s="19"/>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="H7" s="19"/>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="H8" s="19"/>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="H9" s="19"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView showRuler="0" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>67</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView showRuler="0" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>68</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView showRuler="0" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>69</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView showRuler="0" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView showRuler="0" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>71</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView showRuler="0" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>72</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView showRuler="0" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>73</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView showRuler="0" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>74</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView showRuler="0" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>75</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView showRuler="0" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>77</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N81"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="12.33203125" customWidth="1"/>
     <col min="2" max="2" width="13.6640625" customWidth="1"/>
@@ -3675,7 +4071,7 @@
     <col min="13" max="13" width="11.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:14" ht="15">
       <c r="A1" s="4" t="s">
         <v>109</v>
       </c>
@@ -3713,7 +4109,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:14">
       <c r="A2" s="12">
         <v>1</v>
       </c>
@@ -3729,10 +4125,10 @@
       <c r="E2">
         <v>80</v>
       </c>
-      <c r="F2" s="11" t="n">
-        <v>0.638888888888889</v>
-      </c>
-      <c r="G2" s="2" t="n">
+      <c r="F2" s="11">
+        <v>0.63888888888888895</v>
+      </c>
+      <c r="G2" s="2">
         <v>44180</v>
       </c>
       <c r="K2" s="8">
@@ -3748,7 +4144,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:14">
       <c r="A3" s="12">
         <v>2</v>
       </c>
@@ -3764,14 +4160,14 @@
       <c r="E3">
         <v>158</v>
       </c>
-      <c r="F3" s="11" t="n">
-        <v>0.6666666666666666</v>
-      </c>
-      <c r="G3" s="2" t="n">
+      <c r="F3" s="11">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="G3" s="2">
         <v>37305</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:14">
       <c r="A4" s="12">
         <v>3</v>
       </c>
@@ -3787,14 +4183,14 @@
       <c r="E4">
         <v>239</v>
       </c>
-      <c r="F4" s="11" t="n">
-        <v>0.3958333333333333</v>
-      </c>
-      <c r="G4" s="2" t="n">
+      <c r="F4" s="11">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="G4" s="2">
         <v>43907</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:14">
       <c r="A5" s="12">
         <v>4</v>
       </c>
@@ -3810,14 +4206,14 @@
       <c r="E5">
         <v>304</v>
       </c>
-      <c r="F5" s="11" t="n">
+      <c r="F5" s="11">
         <v>0.78125</v>
       </c>
-      <c r="G5" s="2" t="n">
+      <c r="G5" s="2">
         <v>44180</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:14">
       <c r="A6" s="12">
         <v>5</v>
       </c>
@@ -3833,14 +4229,14 @@
       <c r="E6">
         <v>317</v>
       </c>
-      <c r="F6" s="11" t="n">
-        <v>0.7916666666666666</v>
-      </c>
-      <c r="G6" s="2" t="n">
+      <c r="F6" s="11">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="G6" s="2">
         <v>43887</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:14">
       <c r="A7" s="12">
         <v>6</v>
       </c>
@@ -3856,14 +4252,14 @@
       <c r="E7">
         <v>204</v>
       </c>
-      <c r="F7" s="11" t="n">
-        <v>0.9166666666666666</v>
-      </c>
-      <c r="G7" s="2" t="n">
+      <c r="F7" s="11">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="G7" s="2">
         <v>43868</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:14">
       <c r="A8" s="12">
         <v>7</v>
       </c>
@@ -3879,17 +4275,17 @@
       <c r="E8">
         <v>142</v>
       </c>
-      <c r="F8" s="11" t="n">
+      <c r="F8" s="11">
         <v>0.47222222222222227</v>
       </c>
-      <c r="G8" s="2" t="n">
+      <c r="G8" s="2">
         <v>44169</v>
       </c>
       <c r="H8" s="13" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:14">
       <c r="A9" s="12">
         <v>8</v>
       </c>
@@ -3905,14 +4301,14 @@
       <c r="E9">
         <v>306</v>
       </c>
-      <c r="F9" s="11" t="n">
-        <v>0.513888888888889</v>
-      </c>
-      <c r="G9" s="2" t="n">
+      <c r="F9" s="11">
+        <v>0.51388888888888895</v>
+      </c>
+      <c r="G9" s="2">
         <v>44170</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:14">
       <c r="A10" s="12">
         <v>9</v>
       </c>
@@ -3928,14 +4324,14 @@
       <c r="E10">
         <v>270</v>
       </c>
-      <c r="F10" s="11" t="n">
-        <v>0.555555555555556</v>
-      </c>
-      <c r="G10" s="2" t="n">
+      <c r="F10" s="11">
+        <v>0.55555555555555602</v>
+      </c>
+      <c r="G10" s="2">
         <v>44171</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:14">
       <c r="A11" s="12">
         <v>10</v>
       </c>
@@ -3951,14 +4347,14 @@
       <c r="E11">
         <v>96</v>
       </c>
-      <c r="F11" s="11" t="n">
-        <v>0.597222222222222</v>
-      </c>
-      <c r="G11" s="2" t="n">
+      <c r="F11" s="11">
+        <v>0.59722222222222199</v>
+      </c>
+      <c r="G11" s="2">
         <v>44172</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:14">
       <c r="A12" s="12">
         <v>11</v>
       </c>
@@ -3974,14 +4370,14 @@
       <c r="E12">
         <v>371</v>
       </c>
-      <c r="F12" s="11" t="n">
-        <v>0.638888888888889</v>
-      </c>
-      <c r="G12" s="2" t="n">
+      <c r="F12" s="11">
+        <v>0.63888888888888895</v>
+      </c>
+      <c r="G12" s="2">
         <v>44173</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:14">
       <c r="A13" s="12">
         <v>12</v>
       </c>
@@ -3997,14 +4393,14 @@
       <c r="E13">
         <v>229</v>
       </c>
-      <c r="F13" s="11" t="n">
-        <v>0.680555555555556</v>
-      </c>
-      <c r="G13" s="2" t="n">
+      <c r="F13" s="11">
+        <v>0.68055555555555602</v>
+      </c>
+      <c r="G13" s="2">
         <v>44174</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:14">
       <c r="A14" s="12">
         <v>13</v>
       </c>
@@ -4020,14 +4416,14 @@
       <c r="E14">
         <v>209</v>
       </c>
-      <c r="F14" s="11" t="n">
-        <v>0.722222222222222</v>
-      </c>
-      <c r="G14" s="2" t="n">
+      <c r="F14" s="11">
+        <v>0.72222222222222199</v>
+      </c>
+      <c r="G14" s="2">
         <v>44175</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:14">
       <c r="A15" s="12">
         <v>14</v>
       </c>
@@ -4043,14 +4439,14 @@
       <c r="E15">
         <v>311</v>
       </c>
-      <c r="F15" s="11" t="n">
-        <v>0.763888888888889</v>
-      </c>
-      <c r="G15" s="2" t="n">
+      <c r="F15" s="11">
+        <v>0.76388888888888895</v>
+      </c>
+      <c r="G15" s="2">
         <v>44176</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:14">
       <c r="A16" s="12">
         <v>15</v>
       </c>
@@ -4066,14 +4462,14 @@
       <c r="E16">
         <v>290</v>
       </c>
-      <c r="F16" s="11" t="n">
-        <v>0.805555555555556</v>
-      </c>
-      <c r="G16" s="2" t="n">
+      <c r="F16" s="11">
+        <v>0.80555555555555602</v>
+      </c>
+      <c r="G16" s="2">
         <v>44177</v>
       </c>
     </row>
-    <row r="17" spans="1:14">
+    <row r="17" spans="1:7">
       <c r="A17" s="12">
         <v>16</v>
       </c>
@@ -4089,14 +4485,14 @@
       <c r="E17">
         <v>141</v>
       </c>
-      <c r="F17" s="11" t="n">
-        <v>0.847222222222222</v>
-      </c>
-      <c r="G17" s="2" t="n">
+      <c r="F17" s="11">
+        <v>0.84722222222222199</v>
+      </c>
+      <c r="G17" s="2">
         <v>44178</v>
       </c>
     </row>
-    <row r="18" spans="1:14">
+    <row r="18" spans="1:7">
       <c r="A18" s="12">
         <v>17</v>
       </c>
@@ -4112,14 +4508,14 @@
       <c r="E18">
         <v>118</v>
       </c>
-      <c r="F18" s="11" t="n">
-        <v>0.888888888888889</v>
-      </c>
-      <c r="G18" s="2" t="n">
+      <c r="F18" s="11">
+        <v>0.88888888888888895</v>
+      </c>
+      <c r="G18" s="2">
         <v>44179</v>
       </c>
     </row>
-    <row r="19" spans="1:14">
+    <row r="19" spans="1:7">
       <c r="A19" s="12">
         <v>18</v>
       </c>
@@ -4135,14 +4531,14 @@
       <c r="E19">
         <v>192</v>
       </c>
-      <c r="F19" s="11" t="n">
-        <v>0.930555555555556</v>
-      </c>
-      <c r="G19" s="2" t="n">
+      <c r="F19" s="11">
+        <v>0.93055555555555602</v>
+      </c>
+      <c r="G19" s="2">
         <v>44180</v>
       </c>
     </row>
-    <row r="20" spans="1:14">
+    <row r="20" spans="1:7">
       <c r="A20" s="12">
         <v>19</v>
       </c>
@@ -4158,14 +4554,14 @@
       <c r="E20">
         <v>146</v>
       </c>
-      <c r="F20" s="11" t="n">
-        <v>0.972222222222222</v>
-      </c>
-      <c r="G20" s="2" t="n">
+      <c r="F20" s="11">
+        <v>0.97222222222222199</v>
+      </c>
+      <c r="G20" s="2">
         <v>44181</v>
       </c>
     </row>
-    <row r="21" spans="1:14">
+    <row r="21" spans="1:7">
       <c r="A21" s="12">
         <v>20</v>
       </c>
@@ -4181,14 +4577,14 @@
       <c r="E21">
         <v>284</v>
       </c>
-      <c r="F21" s="11" t="n">
-        <v>0.013888888888888888</v>
-      </c>
-      <c r="G21" s="2" t="n">
+      <c r="F21" s="11">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="G21" s="2">
         <v>44182</v>
       </c>
     </row>
-    <row r="22" spans="1:14">
+    <row r="22" spans="1:7">
       <c r="A22" s="12">
         <v>21</v>
       </c>
@@ -4204,14 +4600,14 @@
       <c r="E22">
         <v>323</v>
       </c>
-      <c r="F22" s="11" t="n">
-        <v>0.05555555555555555</v>
-      </c>
-      <c r="G22" s="2" t="n">
+      <c r="F22" s="11">
+        <v>5.5555555555555552E-2</v>
+      </c>
+      <c r="G22" s="2">
         <v>44183</v>
       </c>
     </row>
-    <row r="23" spans="1:14">
+    <row r="23" spans="1:7">
       <c r="A23" s="12">
         <v>22</v>
       </c>
@@ -4227,14 +4623,14 @@
       <c r="E23">
         <v>118</v>
       </c>
-      <c r="F23" s="11" t="n">
-        <v>0.09722222222222222</v>
-      </c>
-      <c r="G23" s="2" t="n">
+      <c r="F23" s="11">
+        <v>9.7222222222222224E-2</v>
+      </c>
+      <c r="G23" s="2">
         <v>44184</v>
       </c>
     </row>
-    <row r="24" spans="1:14">
+    <row r="24" spans="1:7">
       <c r="A24" s="12">
         <v>23</v>
       </c>
@@ -4250,14 +4646,14 @@
       <c r="E24">
         <v>292</v>
       </c>
-      <c r="F24" s="11" t="n">
+      <c r="F24" s="11">
         <v>0.1388888888888889</v>
       </c>
-      <c r="G24" s="2" t="n">
+      <c r="G24" s="2">
         <v>44185</v>
       </c>
     </row>
-    <row r="25" spans="1:14">
+    <row r="25" spans="1:7">
       <c r="A25" s="12">
         <v>24</v>
       </c>
@@ -4273,14 +4669,14 @@
       <c r="E25">
         <v>218</v>
       </c>
-      <c r="F25" s="11" t="n">
+      <c r="F25" s="11">
         <v>0.18055555555555555</v>
       </c>
-      <c r="G25" s="2" t="n">
+      <c r="G25" s="2">
         <v>44186</v>
       </c>
     </row>
-    <row r="26" spans="1:14">
+    <row r="26" spans="1:7">
       <c r="A26" s="12">
         <v>25</v>
       </c>
@@ -4296,14 +4692,14 @@
       <c r="E26">
         <v>205</v>
       </c>
-      <c r="F26" s="11" t="n">
-        <v>0.2222222222222222</v>
-      </c>
-      <c r="G26" s="2" t="n">
+      <c r="F26" s="11">
+        <v>0.22222222222222221</v>
+      </c>
+      <c r="G26" s="2">
         <v>44187</v>
       </c>
     </row>
-    <row r="27" spans="1:14">
+    <row r="27" spans="1:7">
       <c r="A27" s="12">
         <v>26</v>
       </c>
@@ -4319,14 +4715,14 @@
       <c r="E27">
         <v>163</v>
       </c>
-      <c r="F27" s="11" t="n">
+      <c r="F27" s="11">
         <v>0.2638888888888889</v>
       </c>
-      <c r="G27" s="2" t="n">
+      <c r="G27" s="2">
         <v>44188</v>
       </c>
     </row>
-    <row r="28" spans="1:14">
+    <row r="28" spans="1:7">
       <c r="A28" s="12">
         <v>27</v>
       </c>
@@ -4342,14 +4738,14 @@
       <c r="E28">
         <v>196</v>
       </c>
-      <c r="F28" s="11" t="n">
-        <v>0.3055555555555555</v>
-      </c>
-      <c r="G28" s="2" t="n">
+      <c r="F28" s="11">
+        <v>0.30555555555555552</v>
+      </c>
+      <c r="G28" s="2">
         <v>44189</v>
       </c>
     </row>
-    <row r="29" spans="1:14">
+    <row r="29" spans="1:7">
       <c r="A29" s="12">
         <v>28</v>
       </c>
@@ -4365,14 +4761,14 @@
       <c r="E29">
         <v>223</v>
       </c>
-      <c r="F29" s="11" t="n">
+      <c r="F29" s="11">
         <v>0.34722222222222227</v>
       </c>
-      <c r="G29" s="2" t="n">
+      <c r="G29" s="2">
         <v>44190</v>
       </c>
     </row>
-    <row r="30" spans="1:14">
+    <row r="30" spans="1:7">
       <c r="A30" s="12">
         <v>29</v>
       </c>
@@ -4388,14 +4784,14 @@
       <c r="E30">
         <v>367</v>
       </c>
-      <c r="F30" s="11" t="n">
+      <c r="F30" s="11">
         <v>0.3888888888888889</v>
       </c>
-      <c r="G30" s="2" t="n">
+      <c r="G30" s="2">
         <v>44191</v>
       </c>
     </row>
-    <row r="31" spans="1:14">
+    <row r="31" spans="1:7">
       <c r="A31" s="12">
         <v>30</v>
       </c>
@@ -4411,14 +4807,14 @@
       <c r="E31">
         <v>330</v>
       </c>
-      <c r="F31" s="11" t="n">
-        <v>0.4305555555555556</v>
-      </c>
-      <c r="G31" s="2" t="n">
+      <c r="F31" s="11">
+        <v>0.43055555555555558</v>
+      </c>
+      <c r="G31" s="2">
         <v>44192</v>
       </c>
     </row>
-    <row r="32" spans="1:14">
+    <row r="32" spans="1:7">
       <c r="A32" s="12">
         <v>31</v>
       </c>
@@ -4434,10 +4830,10 @@
       <c r="E32">
         <v>181</v>
       </c>
-      <c r="F32" s="11" t="n">
+      <c r="F32" s="11">
         <v>0.47222222222222227</v>
       </c>
-      <c r="G32" s="2" t="n">
+      <c r="G32" s="2">
         <v>44193</v>
       </c>
     </row>
@@ -4457,10 +4853,10 @@
       <c r="E33">
         <v>184</v>
       </c>
-      <c r="F33" s="11" t="n">
-        <v>0.513888888888889</v>
-      </c>
-      <c r="G33" s="2" t="n">
+      <c r="F33" s="11">
+        <v>0.51388888888888895</v>
+      </c>
+      <c r="G33" s="2">
         <v>44194</v>
       </c>
     </row>
@@ -4480,10 +4876,10 @@
       <c r="E34">
         <v>245</v>
       </c>
-      <c r="F34" s="11" t="n">
-        <v>0.5555555555555556</v>
-      </c>
-      <c r="G34" s="2" t="n">
+      <c r="F34" s="11">
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="G34" s="2">
         <v>44195</v>
       </c>
     </row>
@@ -4503,10 +4899,10 @@
       <c r="E35">
         <v>342</v>
       </c>
-      <c r="F35" s="11" t="n">
-        <v>0.5972222222222222</v>
-      </c>
-      <c r="G35" s="2" t="n">
+      <c r="F35" s="11">
+        <v>0.59722222222222221</v>
+      </c>
+      <c r="G35" s="2">
         <v>44196</v>
       </c>
     </row>
@@ -4526,10 +4922,10 @@
       <c r="E36">
         <v>306</v>
       </c>
-      <c r="F36" s="11" t="n">
-        <v>0.638888888888889</v>
-      </c>
-      <c r="G36" s="2" t="n">
+      <c r="F36" s="11">
+        <v>0.63888888888888895</v>
+      </c>
+      <c r="G36" s="2">
         <v>44197</v>
       </c>
     </row>
@@ -4549,10 +4945,10 @@
       <c r="E37">
         <v>190</v>
       </c>
-      <c r="F37" s="11" t="n">
-        <v>0.6805555555555555</v>
-      </c>
-      <c r="G37" s="2" t="n">
+      <c r="F37" s="11">
+        <v>0.68055555555555547</v>
+      </c>
+      <c r="G37" s="2">
         <v>44198</v>
       </c>
     </row>
@@ -4572,10 +4968,10 @@
       <c r="E38">
         <v>282</v>
       </c>
-      <c r="F38" s="11" t="n">
-        <v>0.7222222222222222</v>
-      </c>
-      <c r="G38" s="2" t="n">
+      <c r="F38" s="11">
+        <v>0.72222222222222221</v>
+      </c>
+      <c r="G38" s="2">
         <v>44199</v>
       </c>
     </row>
@@ -4595,10 +4991,10 @@
       <c r="E39">
         <v>232</v>
       </c>
-      <c r="F39" s="11" t="n">
-        <v>0.7638888888888888</v>
-      </c>
-      <c r="G39" s="2" t="n">
+      <c r="F39" s="11">
+        <v>0.76388888888888884</v>
+      </c>
+      <c r="G39" s="2">
         <v>44200</v>
       </c>
     </row>
@@ -4618,10 +5014,10 @@
       <c r="E40">
         <v>155</v>
       </c>
-      <c r="F40" s="11" t="n">
-        <v>0.8055555555555555</v>
-      </c>
-      <c r="G40" s="2" t="n">
+      <c r="F40" s="11">
+        <v>0.80555555555555547</v>
+      </c>
+      <c r="G40" s="2">
         <v>44201</v>
       </c>
     </row>
@@ -4641,10 +5037,10 @@
       <c r="E41">
         <v>320</v>
       </c>
-      <c r="F41" s="11" t="n">
-        <v>0.8472222222222222</v>
-      </c>
-      <c r="G41" s="2" t="n">
+      <c r="F41" s="11">
+        <v>0.84722222222222221</v>
+      </c>
+      <c r="G41" s="2">
         <v>44202</v>
       </c>
     </row>
@@ -4664,10 +5060,10 @@
       <c r="E42">
         <v>150</v>
       </c>
-      <c r="F42" s="11" t="n">
-        <v>0.8888888888888888</v>
-      </c>
-      <c r="G42" s="2" t="n">
+      <c r="F42" s="11">
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="G42" s="2">
         <v>44203</v>
       </c>
     </row>
@@ -4687,10 +5083,10 @@
       <c r="E43">
         <v>236</v>
       </c>
-      <c r="F43" s="11" t="n">
-        <v>0.9305555555555555</v>
-      </c>
-      <c r="G43" s="2" t="n">
+      <c r="F43" s="11">
+        <v>0.93055555555555547</v>
+      </c>
+      <c r="G43" s="2">
         <v>44204</v>
       </c>
     </row>
@@ -4710,10 +5106,10 @@
       <c r="E44">
         <v>293</v>
       </c>
-      <c r="F44" s="11" t="n">
-        <v>0.9722222222222222</v>
-      </c>
-      <c r="G44" s="2" t="n">
+      <c r="F44" s="11">
+        <v>0.97222222222222221</v>
+      </c>
+      <c r="G44" s="2">
         <v>44205</v>
       </c>
     </row>
@@ -4733,10 +5129,10 @@
       <c r="E45">
         <v>101</v>
       </c>
-      <c r="F45" s="11" t="n">
-        <v>0.013888888888888888</v>
-      </c>
-      <c r="G45" s="2" t="n">
+      <c r="F45" s="11">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="G45" s="2">
         <v>44206</v>
       </c>
     </row>
@@ -4756,10 +5152,10 @@
       <c r="E46">
         <v>223</v>
       </c>
-      <c r="F46" s="11" t="n">
-        <v>0.05555555555555555</v>
-      </c>
-      <c r="G46" s="2" t="n">
+      <c r="F46" s="11">
+        <v>5.5555555555555552E-2</v>
+      </c>
+      <c r="G46" s="2">
         <v>44207</v>
       </c>
     </row>
@@ -4779,10 +5175,10 @@
       <c r="E47">
         <v>202</v>
       </c>
-      <c r="F47" s="11" t="n">
-        <v>0.09722222222222222</v>
-      </c>
-      <c r="G47" s="2" t="n">
+      <c r="F47" s="11">
+        <v>9.7222222222222224E-2</v>
+      </c>
+      <c r="G47" s="2">
         <v>44208</v>
       </c>
     </row>
@@ -4802,10 +5198,10 @@
       <c r="E48">
         <v>361</v>
       </c>
-      <c r="F48" s="11" t="n">
+      <c r="F48" s="11">
         <v>0.1388888888888889</v>
       </c>
-      <c r="G48" s="2" t="n">
+      <c r="G48" s="2">
         <v>44209</v>
       </c>
     </row>
@@ -4825,10 +5221,10 @@
       <c r="E49">
         <v>103</v>
       </c>
-      <c r="F49" s="11" t="n">
+      <c r="F49" s="11">
         <v>0.18055555555555555</v>
       </c>
-      <c r="G49" s="2" t="n">
+      <c r="G49" s="2">
         <v>44210</v>
       </c>
     </row>
@@ -4848,10 +5244,10 @@
       <c r="E50">
         <v>379</v>
       </c>
-      <c r="F50" s="11" t="n">
-        <v>0.2222222222222222</v>
-      </c>
-      <c r="G50" s="2" t="n">
+      <c r="F50" s="11">
+        <v>0.22222222222222221</v>
+      </c>
+      <c r="G50" s="2">
         <v>44211</v>
       </c>
     </row>
@@ -4871,10 +5267,10 @@
       <c r="E51">
         <v>309</v>
       </c>
-      <c r="F51" s="11" t="n">
+      <c r="F51" s="11">
         <v>0.2638888888888889</v>
       </c>
-      <c r="G51" s="2" t="n">
+      <c r="G51" s="2">
         <v>44212</v>
       </c>
     </row>
@@ -4894,10 +5290,10 @@
       <c r="E52">
         <v>365</v>
       </c>
-      <c r="F52" s="11" t="n">
-        <v>0.3055555555555555</v>
-      </c>
-      <c r="G52" s="2" t="n">
+      <c r="F52" s="11">
+        <v>0.30555555555555552</v>
+      </c>
+      <c r="G52" s="2">
         <v>44213</v>
       </c>
     </row>
@@ -4917,10 +5313,10 @@
       <c r="E53">
         <v>259</v>
       </c>
-      <c r="F53" s="11" t="n">
+      <c r="F53" s="11">
         <v>0.34722222222222227</v>
       </c>
-      <c r="G53" s="2" t="n">
+      <c r="G53" s="2">
         <v>44214</v>
       </c>
     </row>
@@ -4940,10 +5336,10 @@
       <c r="E54">
         <v>227</v>
       </c>
-      <c r="F54" s="11" t="n">
+      <c r="F54" s="11">
         <v>0.3888888888888889</v>
       </c>
-      <c r="G54" s="2" t="n">
+      <c r="G54" s="2">
         <v>44215</v>
       </c>
     </row>
@@ -4963,10 +5359,10 @@
       <c r="E55">
         <v>105</v>
       </c>
-      <c r="F55" s="11" t="n">
-        <v>0.4305555555555556</v>
-      </c>
-      <c r="G55" s="2" t="n">
+      <c r="F55" s="11">
+        <v>0.43055555555555558</v>
+      </c>
+      <c r="G55" s="2">
         <v>44216</v>
       </c>
     </row>
@@ -4986,10 +5382,10 @@
       <c r="E56">
         <v>151</v>
       </c>
-      <c r="F56" s="11" t="n">
+      <c r="F56" s="11">
         <v>0.47222222222222227</v>
       </c>
-      <c r="G56" s="2" t="n">
+      <c r="G56" s="2">
         <v>44217</v>
       </c>
     </row>
@@ -5009,10 +5405,10 @@
       <c r="E57">
         <v>229</v>
       </c>
-      <c r="F57" s="11" t="n">
-        <v>0.513888888888889</v>
-      </c>
-      <c r="G57" s="2" t="n">
+      <c r="F57" s="11">
+        <v>0.51388888888888895</v>
+      </c>
+      <c r="G57" s="2">
         <v>44218</v>
       </c>
     </row>
@@ -5032,10 +5428,10 @@
       <c r="E58">
         <v>212</v>
       </c>
-      <c r="F58" s="11" t="n">
-        <v>0.5555555555555556</v>
-      </c>
-      <c r="G58" s="2" t="n">
+      <c r="F58" s="11">
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="G58" s="2">
         <v>44219</v>
       </c>
     </row>
@@ -5055,10 +5451,10 @@
       <c r="E59">
         <v>310</v>
       </c>
-      <c r="F59" s="11" t="n">
-        <v>0.5972222222222222</v>
-      </c>
-      <c r="G59" s="2" t="n">
+      <c r="F59" s="11">
+        <v>0.59722222222222221</v>
+      </c>
+      <c r="G59" s="2">
         <v>44220</v>
       </c>
     </row>
@@ -5078,10 +5474,10 @@
       <c r="E60">
         <v>271</v>
       </c>
-      <c r="F60" s="11" t="n">
-        <v>0.638888888888889</v>
-      </c>
-      <c r="G60" s="2" t="n">
+      <c r="F60" s="11">
+        <v>0.63888888888888895</v>
+      </c>
+      <c r="G60" s="2">
         <v>44221</v>
       </c>
     </row>
@@ -5101,10 +5497,10 @@
       <c r="E61">
         <v>347</v>
       </c>
-      <c r="F61" s="11" t="n">
-        <v>0.6805555555555555</v>
-      </c>
-      <c r="G61" s="2" t="n">
+      <c r="F61" s="11">
+        <v>0.68055555555555547</v>
+      </c>
+      <c r="G61" s="2">
         <v>44222</v>
       </c>
     </row>
@@ -5124,10 +5520,10 @@
       <c r="E62">
         <v>351</v>
       </c>
-      <c r="F62" s="11" t="n">
-        <v>0.7222222222222222</v>
-      </c>
-      <c r="G62" s="2" t="n">
+      <c r="F62" s="11">
+        <v>0.72222222222222221</v>
+      </c>
+      <c r="G62" s="2">
         <v>44223</v>
       </c>
     </row>
@@ -5147,10 +5543,10 @@
       <c r="E63">
         <v>143</v>
       </c>
-      <c r="F63" s="11" t="n">
-        <v>0.7638888888888888</v>
-      </c>
-      <c r="G63" s="2" t="n">
+      <c r="F63" s="11">
+        <v>0.76388888888888884</v>
+      </c>
+      <c r="G63" s="2">
         <v>44224</v>
       </c>
     </row>
@@ -5170,10 +5566,10 @@
       <c r="E64">
         <v>140</v>
       </c>
-      <c r="F64" s="11" t="n">
-        <v>0.8055555555555555</v>
-      </c>
-      <c r="G64" s="2" t="n">
+      <c r="F64" s="11">
+        <v>0.80555555555555547</v>
+      </c>
+      <c r="G64" s="2">
         <v>44225</v>
       </c>
     </row>
@@ -5193,10 +5589,10 @@
       <c r="E65">
         <v>87</v>
       </c>
-      <c r="F65" s="11" t="n">
-        <v>0.8472222222222222</v>
-      </c>
-      <c r="G65" s="2" t="n">
+      <c r="F65" s="11">
+        <v>0.84722222222222221</v>
+      </c>
+      <c r="G65" s="2">
         <v>44226</v>
       </c>
     </row>
@@ -5216,10 +5612,10 @@
       <c r="E66">
         <v>132</v>
       </c>
-      <c r="F66" s="11" t="n">
-        <v>0.8888888888888888</v>
-      </c>
-      <c r="G66" s="2" t="n">
+      <c r="F66" s="11">
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="G66" s="2">
         <v>44227</v>
       </c>
     </row>
@@ -5239,10 +5635,10 @@
       <c r="E67">
         <v>333</v>
       </c>
-      <c r="F67" s="11" t="n">
-        <v>0.9305555555555555</v>
-      </c>
-      <c r="G67" s="2" t="n">
+      <c r="F67" s="11">
+        <v>0.93055555555555547</v>
+      </c>
+      <c r="G67" s="2">
         <v>44228</v>
       </c>
     </row>
@@ -5262,10 +5658,10 @@
       <c r="E68">
         <v>141</v>
       </c>
-      <c r="F68" s="11" t="n">
-        <v>0.9722222222222222</v>
-      </c>
-      <c r="G68" s="2" t="n">
+      <c r="F68" s="11">
+        <v>0.97222222222222221</v>
+      </c>
+      <c r="G68" s="2">
         <v>44229</v>
       </c>
     </row>
@@ -5285,10 +5681,10 @@
       <c r="E69">
         <v>99</v>
       </c>
-      <c r="F69" s="11" t="n">
-        <v>0.013888888888888888</v>
-      </c>
-      <c r="G69" s="2" t="n">
+      <c r="F69" s="11">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="G69" s="2">
         <v>44230</v>
       </c>
     </row>
@@ -5308,10 +5704,10 @@
       <c r="E70">
         <v>195</v>
       </c>
-      <c r="F70" s="11" t="n">
-        <v>0.05555555555555555</v>
-      </c>
-      <c r="G70" s="2" t="n">
+      <c r="F70" s="11">
+        <v>5.5555555555555552E-2</v>
+      </c>
+      <c r="G70" s="2">
         <v>44231</v>
       </c>
     </row>
@@ -5331,10 +5727,10 @@
       <c r="E71">
         <v>261</v>
       </c>
-      <c r="F71" s="11" t="n">
-        <v>0.09722222222222222</v>
-      </c>
-      <c r="G71" s="2" t="n">
+      <c r="F71" s="11">
+        <v>9.7222222222222224E-2</v>
+      </c>
+      <c r="G71" s="2">
         <v>44232</v>
       </c>
     </row>
@@ -5354,10 +5750,10 @@
       <c r="E72">
         <v>277</v>
       </c>
-      <c r="F72" s="11" t="n">
+      <c r="F72" s="11">
         <v>0.1388888888888889</v>
       </c>
-      <c r="G72" s="2" t="n">
+      <c r="G72" s="2">
         <v>44233</v>
       </c>
     </row>
@@ -5377,10 +5773,10 @@
       <c r="E73">
         <v>190</v>
       </c>
-      <c r="F73" s="11" t="n">
+      <c r="F73" s="11">
         <v>0.18055555555555555</v>
       </c>
-      <c r="G73" s="2" t="n">
+      <c r="G73" s="2">
         <v>44234</v>
       </c>
     </row>
@@ -5400,10 +5796,10 @@
       <c r="E74">
         <v>88</v>
       </c>
-      <c r="F74" s="11" t="n">
-        <v>0.2222222222222222</v>
-      </c>
-      <c r="G74" s="2" t="n">
+      <c r="F74" s="11">
+        <v>0.22222222222222221</v>
+      </c>
+      <c r="G74" s="2">
         <v>44235</v>
       </c>
     </row>
@@ -5423,10 +5819,10 @@
       <c r="E75">
         <v>278</v>
       </c>
-      <c r="F75" s="11" t="n">
+      <c r="F75" s="11">
         <v>0.2638888888888889</v>
       </c>
-      <c r="G75" s="2" t="n">
+      <c r="G75" s="2">
         <v>44236</v>
       </c>
     </row>
@@ -5446,10 +5842,10 @@
       <c r="E76">
         <v>305</v>
       </c>
-      <c r="F76" s="11" t="n">
-        <v>0.3055555555555555</v>
-      </c>
-      <c r="G76" s="2" t="n">
+      <c r="F76" s="11">
+        <v>0.30555555555555552</v>
+      </c>
+      <c r="G76" s="2">
         <v>44237</v>
       </c>
     </row>
@@ -5469,10 +5865,10 @@
       <c r="E77">
         <v>128</v>
       </c>
-      <c r="F77" s="11" t="n">
+      <c r="F77" s="11">
         <v>0.34722222222222227</v>
       </c>
-      <c r="G77" s="2" t="n">
+      <c r="G77" s="2">
         <v>44238</v>
       </c>
     </row>
@@ -5492,10 +5888,10 @@
       <c r="E78">
         <v>82</v>
       </c>
-      <c r="F78" s="11" t="n">
+      <c r="F78" s="11">
         <v>0.3888888888888889</v>
       </c>
-      <c r="G78" s="2" t="n">
+      <c r="G78" s="2">
         <v>44239</v>
       </c>
     </row>
@@ -5515,10 +5911,10 @@
       <c r="E79">
         <v>403</v>
       </c>
-      <c r="F79" s="15" t="n">
-        <v>0.0715277777777778</v>
-      </c>
-      <c r="G79" s="16" t="n">
+      <c r="F79" s="15">
+        <v>7.1527777777777801E-2</v>
+      </c>
+      <c r="G79" s="16">
         <v>44312</v>
       </c>
     </row>
@@ -5538,15 +5934,15 @@
       <c r="E80">
         <v>457</v>
       </c>
-      <c r="F80" s="15" t="n">
+      <c r="F80" s="15">
         <v>0.109027777777778</v>
       </c>
-      <c r="G80" s="16" t="n">
+      <c r="G80" s="16">
         <v>44312</v>
       </c>
     </row>
     <row r="81" spans="1:7">
-      <c r="A81" t="n">
+      <c r="A81">
         <v>82</v>
       </c>
       <c r="B81" t="s">
@@ -5555,508 +5951,18 @@
       <c r="C81" t="s">
         <v>298</v>
       </c>
-      <c r="D81" t="n">
+      <c r="D81">
         <v>3</v>
       </c>
-      <c r="E81" t="n">
+      <c r="E81">
         <v>459</v>
       </c>
-      <c r="F81" s="15" t="n">
+      <c r="F81" s="15">
         <v>0.110416666666667</v>
       </c>
-      <c r="G81" s="18" t="n">
+      <c r="G81" s="18">
         <v>44312</v>
       </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2">
-        <v>68</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2">
-        <v>69</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2">
-        <v>70</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2">
-        <v>71</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2">
-        <v>72</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2">
-        <v>73</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2">
-        <v>74</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2">
-        <v>75</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
-  <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3">
-        <v>77</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>99</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J31"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="2" max="2" width="9.6640625" customWidth="1"/>
-    <col min="3" max="3" width="9.44140625" customWidth="1"/>
-    <col min="7" max="7" width="10.33203125" customWidth="1"/>
-    <col min="8" max="8" width="6" customWidth="1"/>
-    <col min="9" max="9" width="15.6640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>265</v>
-      </c>
-      <c r="I1" s="14" t="s">
-        <v>264</v>
-      </c>
-      <c r="J1" s="14" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>300</v>
-      </c>
-      <c r="B2" t="s">
-        <v>300</v>
-      </c>
-      <c r="C2" t="s">
-        <v>300</v>
-      </c>
-      <c r="D2" t="s">
-        <v>300</v>
-      </c>
-      <c r="E2" t="s">
-        <v>300</v>
-      </c>
-      <c r="F2" s="15" t="s">
-        <v>300</v>
-      </c>
-      <c r="G2" s="16" t="s">
-        <v>300</v>
-      </c>
-      <c r="H2" t="s">
-        <v>300</v>
-      </c>
-      <c r="I2" t="s">
-        <v>300</v>
-      </c>
-      <c r="J2" t="n">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-    </row>
-    <row r="4">
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-    </row>
-    <row r="5">
-      <c r="F5" s="17"/>
-      <c r="G5" s="17"/>
-    </row>
-    <row r="6">
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
-    </row>
-    <row r="7">
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
-    </row>
-    <row r="8">
-      <c r="F8" s="17"/>
-      <c r="G8" s="17"/>
-    </row>
-    <row r="9">
-      <c r="F9" s="17"/>
-      <c r="G9" s="17"/>
-    </row>
-    <row r="10">
-      <c r="F10" s="17"/>
-      <c r="G10" s="17"/>
-    </row>
-    <row r="11">
-      <c r="F11" s="17"/>
-      <c r="G11" s="17"/>
-    </row>
-    <row r="12">
-      <c r="F12" s="17"/>
-      <c r="G12" s="17"/>
-    </row>
-    <row r="13">
-      <c r="F13" s="17"/>
-      <c r="G13" s="17"/>
-    </row>
-    <row r="14">
-      <c r="F14" s="17"/>
-      <c r="G14" s="17"/>
-    </row>
-    <row r="15">
-      <c r="F15" s="17"/>
-      <c r="G15" s="17"/>
-    </row>
-    <row r="16">
-      <c r="F16" s="17"/>
-      <c r="G16" s="17"/>
-    </row>
-    <row r="17" spans="6:7">
-      <c r="F17" s="17"/>
-      <c r="G17" s="17"/>
-    </row>
-    <row r="18" spans="6:7">
-      <c r="F18" s="17"/>
-      <c r="G18" s="17"/>
-    </row>
-    <row r="19" spans="6:7">
-      <c r="F19" s="17"/>
-      <c r="G19" s="17"/>
-    </row>
-    <row r="20" spans="6:7">
-      <c r="F20" s="17"/>
-      <c r="G20" s="17"/>
-    </row>
-    <row r="21" spans="6:7">
-      <c r="F21" s="17"/>
-      <c r="G21" s="17"/>
-    </row>
-    <row r="22" spans="6:7">
-      <c r="F22" s="17"/>
-      <c r="G22" s="17"/>
-    </row>
-    <row r="23" spans="6:7">
-      <c r="F23" s="17"/>
-      <c r="G23" s="17"/>
-    </row>
-    <row r="24" spans="6:7">
-      <c r="F24" s="17"/>
-      <c r="G24" s="17"/>
-    </row>
-    <row r="25" spans="6:7">
-      <c r="F25" s="17"/>
-      <c r="G25" s="17"/>
-    </row>
-    <row r="26" spans="6:7">
-      <c r="F26" s="17"/>
-      <c r="G26" s="17"/>
-    </row>
-    <row r="27" spans="6:7">
-      <c r="F27" s="17"/>
-      <c r="G27" s="17"/>
-    </row>
-    <row r="28" spans="6:7">
-      <c r="F28" s="17"/>
-      <c r="G28" s="17"/>
-    </row>
-    <row r="29" spans="6:7">
-      <c r="F29" s="17"/>
-      <c r="G29" s="17"/>
-    </row>
-    <row r="30" spans="6:7">
-      <c r="F30" s="17"/>
-      <c r="G30" s="17"/>
-    </row>
-    <row r="31" spans="6:7">
-      <c r="F31" s="17"/>
-      <c r="G31" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6069,7 +5975,7 @@
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="4" t="s">
@@ -6093,7 +5999,7 @@
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="4" t="s">
@@ -6117,7 +6023,7 @@
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="4" t="s">
@@ -6141,7 +6047,7 @@
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="4" t="s">
@@ -6165,7 +6071,7 @@
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="4" t="s">
@@ -6189,7 +6095,7 @@
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="4" t="s">
@@ -6213,7 +6119,7 @@
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="4" t="s">
@@ -6237,7 +6143,7 @@
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="4" t="s">
@@ -6261,7 +6167,7 @@
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="4" t="s">
@@ -6281,59 +6187,21 @@
 
 <file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:3">
       <c r="A1" s="4" t="s">
         <v>97</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>238</v>
+        <v>98</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>239</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>240</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2" t="s">
-        <v>241</v>
-      </c>
-      <c r="E2" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5">
-        <v>14</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -6343,71 +6211,198 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
+    <col min="2" max="2" width="9.6640625" customWidth="1"/>
+    <col min="3" max="3" width="9.44140625" customWidth="1"/>
+    <col min="7" max="7" width="10.33203125" customWidth="1"/>
     <col min="8" max="8" width="6" customWidth="1"/>
+    <col min="9" max="9" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:10">
       <c r="A1" s="4" t="s">
-        <v>97</v>
+        <v>109</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2">
-        <v>1</v>
+        <v>107</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="I1" s="14" t="s">
+        <v>264</v>
+      </c>
+      <c r="J1" s="14" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" t="s">
+        <v>299</v>
       </c>
       <c r="B2" t="s">
-        <v>237</v>
+        <v>299</v>
       </c>
       <c r="C2" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4">
-        <v>78</v>
-      </c>
-      <c r="B4" t="s">
-        <v>260</v>
-      </c>
-      <c r="C4" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5">
-        <v>80</v>
-      </c>
-      <c r="B5" t="s">
-        <v>298</v>
-      </c>
-      <c r="C5" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="n">
-        <v>82</v>
-      </c>
+        <v>299</v>
+      </c>
+      <c r="D2" t="s">
+        <v>299</v>
+      </c>
+      <c r="E2" t="s">
+        <v>299</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>299</v>
+      </c>
+      <c r="G2" s="16" t="s">
+        <v>299</v>
+      </c>
+      <c r="H2" t="s">
+        <v>299</v>
+      </c>
+      <c r="I2" t="s">
+        <v>299</v>
+      </c>
+      <c r="J2">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="F11" s="17"/>
+      <c r="G11" s="17"/>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="F12" s="17"/>
+      <c r="G12" s="17"/>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="F13" s="17"/>
+      <c r="G13" s="17"/>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
+    </row>
+    <row r="17" spans="6:7">
+      <c r="F17" s="17"/>
+      <c r="G17" s="17"/>
+    </row>
+    <row r="18" spans="6:7">
+      <c r="F18" s="17"/>
+      <c r="G18" s="17"/>
+    </row>
+    <row r="19" spans="6:7">
+      <c r="F19" s="17"/>
+      <c r="G19" s="17"/>
+    </row>
+    <row r="20" spans="6:7">
+      <c r="F20" s="17"/>
+      <c r="G20" s="17"/>
+    </row>
+    <row r="21" spans="6:7">
+      <c r="F21" s="17"/>
+      <c r="G21" s="17"/>
+    </row>
+    <row r="22" spans="6:7">
+      <c r="F22" s="17"/>
+      <c r="G22" s="17"/>
+    </row>
+    <row r="23" spans="6:7">
+      <c r="F23" s="17"/>
+      <c r="G23" s="17"/>
+    </row>
+    <row r="24" spans="6:7">
+      <c r="F24" s="17"/>
+      <c r="G24" s="17"/>
+    </row>
+    <row r="25" spans="6:7">
+      <c r="F25" s="17"/>
+      <c r="G25" s="17"/>
+    </row>
+    <row r="26" spans="6:7">
+      <c r="F26" s="17"/>
+      <c r="G26" s="17"/>
+    </row>
+    <row r="27" spans="6:7">
+      <c r="F27" s="17"/>
+      <c r="G27" s="17"/>
+    </row>
+    <row r="28" spans="6:7">
+      <c r="F28" s="17"/>
+      <c r="G28" s="17"/>
+    </row>
+    <row r="29" spans="6:7">
+      <c r="F29" s="17"/>
+      <c r="G29" s="17"/>
+    </row>
+    <row r="30" spans="6:7">
+      <c r="F30" s="17"/>
+      <c r="G30" s="17"/>
+    </row>
+    <row r="31" spans="6:7">
+      <c r="F31" s="17"/>
+      <c r="G31" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6420,7 +6415,7 @@
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="4" t="s">
@@ -6441,34 +6436,34 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>253</v>
+        <v>240</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -6478,11 +6473,11 @@
 
 <file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="4" t="s">
@@ -6503,29 +6498,34 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4">
-        <v>12</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -6535,11 +6535,11 @@
 
 <file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="4" t="s">
@@ -6560,49 +6560,29 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" t="n">
-        <v>82</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -6612,11 +6592,11 @@
 
 <file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="4" t="s">
@@ -6637,29 +6617,49 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E2" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3">
-        <v>30</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4">
-        <v>32</v>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8">
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -6673,7 +6673,64 @@
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2">
+        <v>29</v>
+      </c>
+      <c r="B2" t="s">
+        <v>256</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>245</v>
+      </c>
+      <c r="E2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet55.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView showRuler="0" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="4" t="s">
@@ -6726,11 +6783,14 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="8" max="8" width="6" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="4" t="s">
@@ -6745,18 +6805,48 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="C2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3">
-        <v>4</v>
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>78</v>
+      </c>
+      <c r="B4" t="s">
+        <v>260</v>
+      </c>
+      <c r="C4" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>80</v>
+      </c>
+      <c r="B5" t="s">
+        <v>298</v>
+      </c>
+      <c r="C5" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6">
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -6766,11 +6856,11 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="4" t="s">
@@ -6785,22 +6875,18 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>235</v>
+      </c>
+      <c r="C2" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -6810,11 +6896,11 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="4" t="s">
@@ -6829,7 +6915,22 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2">
-        <v>9</v>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -6843,7 +6944,7 @@
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="4" t="s">
@@ -6858,7 +6959,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add: blocking and unblocking people
</commit_message>
<xml_diff>
--- a/build-PSS_HomeWork4-Desktop_Qt_5_12_5_MinGW_64_bit-Release/release/DataBase/Accounts.xlsx
+++ b/build-PSS_HomeWork4-Desktop_Qt_5_12_5_MinGW_64_bit-Release/release/DataBase/Accounts.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660" firstSheet="46" activeTab="52"/>
+    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Passenger" sheetId="1" r:id="rId1"/>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="305">
   <si>
     <t>Leroy</t>
   </si>
@@ -984,9 +984,6 @@
     <t>st. Raisoveta, 8</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>Admin</t>
   </si>
   <si>
@@ -1000,6 +997,9 @@
   </si>
   <si>
     <t>grey</t>
+  </si>
+  <si>
+    <t>Blocked</t>
   </si>
 </sst>
 </file>
@@ -1182,7 +1182,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1209,8 +1209,9 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -1505,11 +1506,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H45"/>
+  <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
@@ -1524,7 +1523,7 @@
     <col min="9" max="9" width="10.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="A1" s="3" t="s">
         <v>87</v>
       </c>
@@ -1549,8 +1548,11 @@
       <c r="H1" s="1" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="2" spans="1:8">
+      <c r="I1" s="18" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>262</v>
       </c>
@@ -1575,8 +1577,11 @@
       <c r="H2">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:8">
+      <c r="I2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -1601,8 +1606,11 @@
       <c r="H3">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:8">
+      <c r="I3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -1627,8 +1635,11 @@
       <c r="H4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:8">
+      <c r="I4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -1653,8 +1664,11 @@
       <c r="H5">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:8">
+      <c r="I5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -1679,8 +1693,11 @@
       <c r="H6">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:8">
+      <c r="I6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -1705,8 +1722,11 @@
       <c r="H7">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:8">
+      <c r="I7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -1731,8 +1751,11 @@
       <c r="H8">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="1:8">
+      <c r="I8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -1757,8 +1780,11 @@
       <c r="H9">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:8">
+      <c r="I9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -1783,8 +1809,11 @@
       <c r="H10">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="1:8">
+      <c r="I10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -1809,8 +1838,11 @@
       <c r="H11">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="1:8">
+      <c r="I11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -1835,8 +1867,11 @@
       <c r="H12">
         <v>3</v>
       </c>
-    </row>
-    <row r="13" spans="1:8">
+      <c r="I12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -1861,8 +1896,11 @@
       <c r="H13">
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="1:8">
+      <c r="I13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
       <c r="A14" t="s">
         <v>1</v>
       </c>
@@ -1887,8 +1925,11 @@
       <c r="H14">
         <v>5</v>
       </c>
-    </row>
-    <row r="15" spans="1:8">
+      <c r="I14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
       <c r="A15" t="s">
         <v>10</v>
       </c>
@@ -1913,8 +1954,11 @@
       <c r="H15">
         <v>5</v>
       </c>
-    </row>
-    <row r="16" spans="1:8">
+      <c r="I15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
       <c r="A16" t="s">
         <v>11</v>
       </c>
@@ -1939,8 +1983,11 @@
       <c r="H16">
         <v>3</v>
       </c>
-    </row>
-    <row r="17" spans="1:8">
+      <c r="I16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
       <c r="A17" t="s">
         <v>12</v>
       </c>
@@ -1965,8 +2012,11 @@
       <c r="H17">
         <v>4</v>
       </c>
-    </row>
-    <row r="18" spans="1:8">
+      <c r="I17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
       <c r="A18" t="s">
         <v>13</v>
       </c>
@@ -1991,8 +2041,11 @@
       <c r="H18">
         <v>2</v>
       </c>
-    </row>
-    <row r="19" spans="1:8">
+      <c r="I18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
       <c r="A19" t="s">
         <v>14</v>
       </c>
@@ -2017,8 +2070,11 @@
       <c r="H19">
         <v>4</v>
       </c>
-    </row>
-    <row r="20" spans="1:8">
+      <c r="I19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
       <c r="A20" t="s">
         <v>15</v>
       </c>
@@ -2043,8 +2099,11 @@
       <c r="H20">
         <v>5</v>
       </c>
-    </row>
-    <row r="21" spans="1:8">
+      <c r="I20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
       <c r="A21" t="s">
         <v>16</v>
       </c>
@@ -2069,8 +2128,11 @@
       <c r="H21">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:8">
+      <c r="I21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
       <c r="A22" t="s">
         <v>17</v>
       </c>
@@ -2095,8 +2157,11 @@
       <c r="H22">
         <v>4</v>
       </c>
-    </row>
-    <row r="23" spans="1:8">
+      <c r="I22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
       <c r="A23" t="s">
         <v>18</v>
       </c>
@@ -2121,8 +2186,11 @@
       <c r="H23">
         <v>5</v>
       </c>
-    </row>
-    <row r="24" spans="1:8">
+      <c r="I23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
       <c r="A24" t="s">
         <v>19</v>
       </c>
@@ -2147,8 +2215,11 @@
       <c r="H24">
         <v>4</v>
       </c>
-    </row>
-    <row r="25" spans="1:8">
+      <c r="I24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
       <c r="A25" t="s">
         <v>20</v>
       </c>
@@ -2173,8 +2244,11 @@
       <c r="H25">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:8">
+      <c r="I25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
       <c r="A26" t="s">
         <v>21</v>
       </c>
@@ -2199,8 +2273,11 @@
       <c r="H26">
         <v>3</v>
       </c>
-    </row>
-    <row r="27" spans="1:8">
+      <c r="I26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
       <c r="A27" t="s">
         <v>22</v>
       </c>
@@ -2225,8 +2302,11 @@
       <c r="H27">
         <v>5</v>
       </c>
-    </row>
-    <row r="28" spans="1:8">
+      <c r="I27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
       <c r="A28" t="s">
         <v>23</v>
       </c>
@@ -2251,8 +2331,11 @@
       <c r="H28">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:8">
+      <c r="I28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
       <c r="A29" t="s">
         <v>24</v>
       </c>
@@ -2277,8 +2360,11 @@
       <c r="H29">
         <v>5</v>
       </c>
-    </row>
-    <row r="30" spans="1:8">
+      <c r="I29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
       <c r="A30" t="s">
         <v>25</v>
       </c>
@@ -2303,8 +2389,11 @@
       <c r="H30">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:8">
+      <c r="I30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
       <c r="A31" t="s">
         <v>26</v>
       </c>
@@ -2329,8 +2418,11 @@
       <c r="H31">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:8">
+      <c r="I31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
       <c r="A32" t="s">
         <v>27</v>
       </c>
@@ -2355,8 +2447,11 @@
       <c r="H32">
         <v>2</v>
       </c>
-    </row>
-    <row r="33" spans="1:8">
+      <c r="I32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
       <c r="A33" t="s">
         <v>28</v>
       </c>
@@ -2381,8 +2476,11 @@
       <c r="H33">
         <v>2</v>
       </c>
-    </row>
-    <row r="34" spans="1:8">
+      <c r="I33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
       <c r="A34" t="s">
         <v>29</v>
       </c>
@@ -2407,8 +2505,11 @@
       <c r="H34">
         <v>2</v>
       </c>
-    </row>
-    <row r="35" spans="1:8">
+      <c r="I34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9">
       <c r="A35" t="s">
         <v>30</v>
       </c>
@@ -2433,8 +2534,11 @@
       <c r="H35">
         <v>5</v>
       </c>
-    </row>
-    <row r="36" spans="1:8">
+      <c r="I35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9">
       <c r="A36" t="s">
         <v>31</v>
       </c>
@@ -2459,8 +2563,11 @@
       <c r="H36">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:8">
+      <c r="I36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9">
       <c r="A37" t="s">
         <v>32</v>
       </c>
@@ -2485,8 +2592,11 @@
       <c r="H37">
         <v>3</v>
       </c>
-    </row>
-    <row r="38" spans="1:8">
+      <c r="I37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9">
       <c r="A38" t="s">
         <v>33</v>
       </c>
@@ -2511,8 +2621,11 @@
       <c r="H38">
         <v>2</v>
       </c>
-    </row>
-    <row r="39" spans="1:8">
+      <c r="I38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9">
       <c r="A39" t="s">
         <v>34</v>
       </c>
@@ -2537,8 +2650,11 @@
       <c r="H39">
         <v>4</v>
       </c>
-    </row>
-    <row r="40" spans="1:8">
+      <c r="I39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9">
       <c r="A40" t="s">
         <v>35</v>
       </c>
@@ -2563,8 +2679,11 @@
       <c r="H40">
         <v>3</v>
       </c>
-    </row>
-    <row r="41" spans="1:8">
+      <c r="I40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9">
       <c r="A41" t="s">
         <v>36</v>
       </c>
@@ -2589,8 +2708,11 @@
       <c r="H41">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="1:8">
+      <c r="I41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9">
       <c r="A42" t="s">
         <v>37</v>
       </c>
@@ -2615,8 +2737,11 @@
       <c r="H42">
         <v>4</v>
       </c>
-    </row>
-    <row r="43" spans="1:8">
+      <c r="I42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9">
       <c r="A43" t="s">
         <v>38</v>
       </c>
@@ -2641,8 +2766,11 @@
       <c r="H43">
         <v>4</v>
       </c>
-    </row>
-    <row r="44" spans="1:8">
+      <c r="I43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9">
       <c r="A44" t="s">
         <v>2</v>
       </c>
@@ -2667,8 +2795,11 @@
       <c r="H44">
         <v>5</v>
       </c>
-    </row>
-    <row r="45" spans="1:8">
+      <c r="I44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9">
       <c r="A45" t="s">
         <v>44</v>
       </c>
@@ -2691,6 +2822,9 @@
         <v>89286091054</v>
       </c>
       <c r="H45">
+        <v>1</v>
+      </c>
+      <c r="I45">
         <v>1</v>
       </c>
     </row>
@@ -2703,7 +2837,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="C1" workbookViewId="0"/>
+    <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
@@ -3071,9 +3205,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
@@ -3084,7 +3220,7 @@
     <col min="8" max="8" width="6.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>87</v>
       </c>
@@ -3109,8 +3245,11 @@
       <c r="H1" s="1" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="2" spans="1:8">
+      <c r="I1" s="18" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>36</v>
       </c>
@@ -3133,10 +3272,13 @@
         <v>333223827</v>
       </c>
       <c r="H2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
+        <v>5</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>39</v>
       </c>
@@ -3161,8 +3303,11 @@
       <c r="H3">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:8">
+      <c r="I3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
         <v>40</v>
       </c>
@@ -3187,8 +3332,11 @@
       <c r="H4">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:8">
+      <c r="I4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
         <v>41</v>
       </c>
@@ -3213,8 +3361,11 @@
       <c r="H5">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:8">
+      <c r="I5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
         <v>42</v>
       </c>
@@ -3237,10 +3388,13 @@
         <v>333227531</v>
       </c>
       <c r="H6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" t="s">
         <v>43</v>
       </c>
@@ -3264,6 +3418,9 @@
       </c>
       <c r="H7">
         <v>4</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -3663,18 +3820,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:7">
       <c r="A1" s="3" t="s">
         <v>87</v>
       </c>
@@ -3696,14 +3851,13 @@
       <c r="G1" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="H1" s="19"/>
-    </row>
-    <row r="2" spans="1:8">
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
+        <v>299</v>
+      </c>
+      <c r="B2" t="s">
         <v>300</v>
-      </c>
-      <c r="B2" t="s">
-        <v>301</v>
       </c>
       <c r="C2" t="s">
         <v>90</v>
@@ -3711,7 +3865,7 @@
       <c r="D2" s="2">
         <v>31257</v>
       </c>
-      <c r="E2" s="19">
+      <c r="E2">
         <v>4223</v>
       </c>
       <c r="F2">
@@ -3720,42 +3874,10 @@
       <c r="G2">
         <v>3377722</v>
       </c>
-      <c r="H2" s="19"/>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="19"/>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="F5" s="19"/>
-      <c r="G5" s="19"/>
-      <c r="H5" s="19"/>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="H6" s="19"/>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="H7" s="19"/>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="H8" s="19"/>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="H9" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
 </file>
 
@@ -4063,7 +4185,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N81"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
@@ -5969,7 +6091,7 @@
       <c r="F81" s="15">
         <v>0.110416666666667</v>
       </c>
-      <c r="G81" s="18">
+      <c r="G81" s="16">
         <v>44312</v>
       </c>
     </row>
@@ -6222,7 +6344,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N11" sqref="N11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
@@ -6266,33 +6390,8 @@
       </c>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" t="s">
-        <v>299</v>
-      </c>
-      <c r="B2" t="s">
-        <v>299</v>
-      </c>
-      <c r="C2" t="s">
-        <v>299</v>
-      </c>
-      <c r="D2" t="s">
-        <v>299</v>
-      </c>
-      <c r="E2" t="s">
-        <v>299</v>
-      </c>
-      <c r="F2" s="15" t="s">
-        <v>299</v>
-      </c>
-      <c r="G2" s="16" t="s">
-        <v>299</v>
-      </c>
-      <c r="H2" t="s">
-        <v>299</v>
-      </c>
-      <c r="I2" t="s">
-        <v>299</v>
-      </c>
+      <c r="F2" s="15"/>
+      <c r="G2" s="16"/>
       <c r="J2">
         <v>83</v>
       </c>
@@ -6603,9 +6702,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
-    </sheetView>
+    <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
@@ -6648,16 +6745,16 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
+        <v>302</v>
+      </c>
+      <c r="E3" t="s">
         <v>303</v>
-      </c>
-      <c r="E3" t="s">
-        <v>304</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -6751,9 +6848,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="E2" sqref="B2:E2"/>
-    </sheetView>
+    <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>

</xml_diff>

<commit_message>
Added ability to verify machines
</commit_message>
<xml_diff>
--- a/build-PSS_HomeWork4-Desktop_Qt_5_12_5_MinGW_64_bit-Release/release/DataBase/Accounts.xlsx
+++ b/build-PSS_HomeWork4-Desktop_Qt_5_12_5_MinGW_64_bit-Release/release/DataBase/Accounts.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660" firstSheet="46" activeTab="52"/>
   </bookViews>
   <sheets>
     <sheet name="Passenger" sheetId="1" r:id="rId1"/>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="306">
   <si>
     <t>Leroy</t>
   </si>
@@ -1000,6 +1000,9 @@
   </si>
   <si>
     <t>Blocked</t>
+  </si>
+  <si>
+    <t>Verified</t>
   </si>
 </sst>
 </file>
@@ -3207,9 +3210,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
@@ -3822,7 +3823,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
@@ -3877,7 +3880,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
 </file>
 
@@ -4185,7 +4187,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
@@ -6344,9 +6346,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
@@ -6519,13 +6519,13 @@
 
 <file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" s="4" t="s">
         <v>97</v>
       </c>
@@ -6541,8 +6541,11 @@
       <c r="E1" s="4" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="14" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>1</v>
       </c>
@@ -6558,18 +6561,21 @@
       <c r="E2" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="F2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:6">
       <c r="A5">
         <v>14</v>
       </c>
@@ -6581,13 +6587,13 @@
 
 <file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" s="4" t="s">
         <v>97</v>
       </c>
@@ -6603,8 +6609,11 @@
       <c r="E1" s="4" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="14" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>2</v>
       </c>
@@ -6620,18 +6629,21 @@
       <c r="E2" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="F2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:6">
       <c r="A5">
         <v>13</v>
       </c>
@@ -6643,13 +6655,13 @@
 
 <file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" s="4" t="s">
         <v>97</v>
       </c>
@@ -6665,8 +6677,11 @@
       <c r="E1" s="4" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="14" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>4</v>
       </c>
@@ -6682,13 +6697,16 @@
       <c r="E2" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="F2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>12</v>
       </c>
@@ -6700,13 +6718,13 @@
 
 <file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" s="4" t="s">
         <v>97</v>
       </c>
@@ -6722,8 +6740,11 @@
       <c r="E1" s="4" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="14" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>3</v>
       </c>
@@ -6739,8 +6760,11 @@
       <c r="E2" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="F2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>5</v>
       </c>
@@ -6756,28 +6780,31 @@
       <c r="E3" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="F3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:6">
       <c r="A5">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:6">
       <c r="A6">
         <v>78</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:6">
       <c r="A7">
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:6">
       <c r="A8">
         <v>82</v>
       </c>
@@ -6789,13 +6816,13 @@
 
 <file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" s="4" t="s">
         <v>97</v>
       </c>
@@ -6811,8 +6838,11 @@
       <c r="E1" s="4" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="14" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>29</v>
       </c>
@@ -6828,13 +6858,16 @@
       <c r="E2" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="F2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>32</v>
       </c>
@@ -6846,13 +6879,15 @@
 
 <file path=xl/worksheets/sheet55.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" s="4" t="s">
         <v>97</v>
       </c>
@@ -6868,8 +6903,11 @@
       <c r="E1" s="4" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="14" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>53</v>
       </c>
@@ -6885,15 +6923,8 @@
       <c r="E2" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4">
-        <v>55</v>
+      <c r="F2">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>